<commit_message>
small adjustment to pull through AL-CASHO
</commit_message>
<xml_diff>
--- a/Earliest_Pay_Rate_Changes.xlsx
+++ b/Earliest_Pay_Rate_Changes.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="107">
   <si>
     <t>Code_</t>
   </si>
@@ -696,7 +696,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C266"/>
+  <dimension ref="A1:C299"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -982,40 +982,40 @@
         <v>14</v>
       </c>
       <c r="B26">
-        <v>32</v>
+        <v>486.4</v>
       </c>
       <c r="C26" s="2">
-        <v>44954</v>
+        <v>44947</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B27">
-        <v>44.65</v>
+        <v>706.8</v>
       </c>
       <c r="C27" s="2">
-        <v>44744</v>
+        <v>44947</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B28">
-        <v>47.17</v>
+        <v>32</v>
       </c>
       <c r="C28" s="2">
-        <v>45059</v>
+        <v>44954</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B29">
-        <v>47.95</v>
+        <v>44.65</v>
       </c>
       <c r="C29" s="2">
         <v>44744</v>
@@ -1023,13 +1023,13 @@
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B30">
-        <v>23.77</v>
+        <v>47.17</v>
       </c>
       <c r="C30" s="2">
-        <v>44751</v>
+        <v>45059</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -1037,51 +1037,51 @@
         <v>16</v>
       </c>
       <c r="B31">
-        <v>22.66</v>
+        <v>47.95</v>
       </c>
       <c r="C31" s="2">
-        <v>45087</v>
+        <v>44744</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B32">
-        <v>27</v>
+        <v>23.77</v>
       </c>
       <c r="C32" s="2">
-        <v>44744</v>
+        <v>44751</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B33">
-        <v>17.86</v>
+        <v>22.66</v>
       </c>
       <c r="C33" s="2">
-        <v>44744</v>
+        <v>45087</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B34">
-        <v>18.76</v>
+        <v>27</v>
       </c>
       <c r="C34" s="2">
-        <v>44751</v>
+        <v>44744</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B35">
-        <v>29.27</v>
+        <v>17.86</v>
       </c>
       <c r="C35" s="2">
         <v>44744</v>
@@ -1089,112 +1089,112 @@
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B36">
-        <v>32.3</v>
+        <v>18.76</v>
       </c>
       <c r="C36" s="2">
-        <v>44835</v>
+        <v>44751</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B37">
-        <v>32</v>
+        <v>29.27</v>
       </c>
       <c r="C37" s="2">
-        <v>44779</v>
+        <v>44744</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B38">
-        <v>45.42</v>
+        <v>32.3</v>
       </c>
       <c r="C38" s="2">
-        <v>44744</v>
+        <v>44835</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B39">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C39" s="2">
-        <v>44744</v>
+        <v>44779</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B40">
-        <v>31.5</v>
+        <v>45.42</v>
       </c>
       <c r="C40" s="2">
-        <v>44835</v>
+        <v>44744</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B41">
-        <v>15.88</v>
+        <v>30</v>
       </c>
       <c r="C41" s="2">
-        <v>44779</v>
+        <v>44744</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B42">
-        <v>18.76</v>
+        <v>31.5</v>
       </c>
       <c r="C42" s="2">
-        <v>44898</v>
+        <v>44835</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B43">
-        <v>50.47</v>
+        <v>15.88</v>
       </c>
       <c r="C43" s="2">
-        <v>44744</v>
+        <v>44779</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B44">
-        <v>26</v>
+        <v>18.76</v>
       </c>
       <c r="C44" s="2">
-        <v>44751</v>
+        <v>44898</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B45">
-        <v>26.73</v>
+        <v>50.47</v>
       </c>
       <c r="C45" s="2">
-        <v>44765</v>
+        <v>44744</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -1202,32 +1202,32 @@
         <v>25</v>
       </c>
       <c r="B46">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C46" s="2">
-        <v>44835</v>
+        <v>44751</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B47">
-        <v>22.73</v>
+        <v>26.73</v>
       </c>
       <c r="C47" s="2">
-        <v>44744</v>
+        <v>44765</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B48">
-        <v>23.77</v>
+        <v>29</v>
       </c>
       <c r="C48" s="2">
-        <v>44758</v>
+        <v>44835</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -1235,32 +1235,32 @@
         <v>26</v>
       </c>
       <c r="B49">
-        <v>24.59</v>
+        <v>22.73</v>
       </c>
       <c r="C49" s="2">
-        <v>44828</v>
+        <v>44744</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B50">
-        <v>26</v>
+        <v>23.77</v>
       </c>
       <c r="C50" s="2">
-        <v>44744</v>
+        <v>44758</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B51">
-        <v>30</v>
+        <v>24.59</v>
       </c>
       <c r="C51" s="2">
-        <v>44744</v>
+        <v>44828</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -1268,7 +1268,7 @@
         <v>27</v>
       </c>
       <c r="B52">
-        <v>41.8</v>
+        <v>26</v>
       </c>
       <c r="C52" s="2">
         <v>44744</v>
@@ -1279,10 +1279,10 @@
         <v>27</v>
       </c>
       <c r="B53">
-        <v>26.73</v>
+        <v>30</v>
       </c>
       <c r="C53" s="2">
-        <v>44751</v>
+        <v>44744</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -1290,10 +1290,10 @@
         <v>27</v>
       </c>
       <c r="B54">
-        <v>28.07</v>
+        <v>41.8</v>
       </c>
       <c r="C54" s="2">
-        <v>44835</v>
+        <v>44744</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -1301,43 +1301,43 @@
         <v>27</v>
       </c>
       <c r="B55">
-        <v>32</v>
+        <v>26.73</v>
       </c>
       <c r="C55" s="2">
-        <v>44961</v>
+        <v>44751</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B56">
-        <v>35</v>
+        <v>28.07</v>
       </c>
       <c r="C56" s="2">
-        <v>44744</v>
+        <v>44835</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B57">
-        <v>22.73</v>
+        <v>32</v>
       </c>
       <c r="C57" s="2">
-        <v>44744</v>
+        <v>44961</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B58">
-        <v>23.77</v>
+        <v>35</v>
       </c>
       <c r="C58" s="2">
-        <v>44751</v>
+        <v>44744</v>
       </c>
     </row>
     <row r="59" spans="1:3">
@@ -1345,73 +1345,73 @@
         <v>29</v>
       </c>
       <c r="B59">
-        <v>24.59</v>
+        <v>22.73</v>
       </c>
       <c r="C59" s="2">
-        <v>44954</v>
+        <v>44744</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B60">
-        <v>12.38</v>
+        <v>23.77</v>
       </c>
       <c r="C60" s="2">
-        <v>44870</v>
+        <v>44751</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B61">
-        <v>30</v>
+        <v>380.32</v>
       </c>
       <c r="C61" s="2">
-        <v>44744</v>
+        <v>44947</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B62">
-        <v>34</v>
+        <v>525.24</v>
       </c>
       <c r="C62" s="2">
-        <v>44744</v>
+        <v>44947</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B63">
-        <v>36</v>
+        <v>24.59</v>
       </c>
       <c r="C63" s="2">
-        <v>44800</v>
+        <v>44954</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B64">
-        <v>31.5</v>
+        <v>12.38</v>
       </c>
       <c r="C64" s="2">
-        <v>44835</v>
+        <v>44870</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B65">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C65" s="2">
         <v>44744</v>
@@ -1419,10 +1419,10 @@
     </row>
     <row r="66" spans="1:3">
       <c r="A66" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B66">
-        <v>60.56</v>
+        <v>34</v>
       </c>
       <c r="C66" s="2">
         <v>44744</v>
@@ -1430,21 +1430,21 @@
     </row>
     <row r="67" spans="1:3">
       <c r="A67" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B67">
-        <v>37.4</v>
+        <v>36</v>
       </c>
       <c r="C67" s="2">
-        <v>44835</v>
+        <v>44800</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B68">
-        <v>65.61</v>
+        <v>31.5</v>
       </c>
       <c r="C68" s="2">
         <v>44835</v>
@@ -1452,90 +1452,90 @@
     </row>
     <row r="69" spans="1:3">
       <c r="A69" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B69">
-        <v>65.61</v>
+        <v>34</v>
       </c>
       <c r="C69" s="2">
-        <v>44940</v>
+        <v>44744</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B70">
-        <v>15.88</v>
+        <v>60.56</v>
       </c>
       <c r="C70" s="2">
-        <v>44961</v>
+        <v>44744</v>
       </c>
     </row>
     <row r="71" spans="1:3">
       <c r="A71" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B71">
-        <v>18.76</v>
+        <v>37.4</v>
       </c>
       <c r="C71" s="2">
-        <v>44975</v>
+        <v>44835</v>
       </c>
     </row>
     <row r="72" spans="1:3">
       <c r="A72" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B72">
-        <v>16.34</v>
+        <v>65.61</v>
       </c>
       <c r="C72" s="2">
-        <v>45087</v>
+        <v>44835</v>
       </c>
     </row>
     <row r="73" spans="1:3">
       <c r="A73" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B73">
-        <v>23.38</v>
+        <v>65.61</v>
       </c>
       <c r="C73" s="2">
-        <v>44744</v>
+        <v>44940</v>
       </c>
     </row>
     <row r="74" spans="1:3">
       <c r="A74" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B74">
-        <v>37</v>
+        <v>15.88</v>
       </c>
       <c r="C74" s="2">
-        <v>44744</v>
+        <v>44961</v>
       </c>
     </row>
     <row r="75" spans="1:3">
       <c r="A75" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B75">
-        <v>24.59</v>
+        <v>18.76</v>
       </c>
       <c r="C75" s="2">
-        <v>44751</v>
+        <v>44975</v>
       </c>
     </row>
     <row r="76" spans="1:3">
       <c r="A76" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B76">
-        <v>45.55</v>
+        <v>16.34</v>
       </c>
       <c r="C76" s="2">
-        <v>44751</v>
+        <v>45087</v>
       </c>
     </row>
     <row r="77" spans="1:3">
@@ -1543,106 +1543,106 @@
         <v>34</v>
       </c>
       <c r="B77">
-        <v>50.97</v>
+        <v>23.38</v>
       </c>
       <c r="C77" s="2">
-        <v>44835</v>
+        <v>44744</v>
       </c>
     </row>
     <row r="78" spans="1:3">
       <c r="A78" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B78">
-        <v>12.99</v>
+        <v>37</v>
       </c>
       <c r="C78" s="2">
-        <v>44793</v>
+        <v>44744</v>
       </c>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B79">
-        <v>15.88</v>
+        <v>24.59</v>
       </c>
       <c r="C79" s="2">
-        <v>44800</v>
+        <v>44751</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B80">
-        <v>17.5</v>
+        <v>45.55</v>
       </c>
       <c r="C80" s="2">
-        <v>44940</v>
+        <v>44751</v>
       </c>
     </row>
     <row r="81" spans="1:3">
       <c r="A81" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B81">
-        <v>30</v>
+        <v>50.97</v>
       </c>
       <c r="C81" s="2">
-        <v>44744</v>
+        <v>44835</v>
       </c>
     </row>
     <row r="82" spans="1:3">
       <c r="A82" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B82">
-        <v>31.5</v>
+        <v>98.36</v>
       </c>
       <c r="C82" s="2">
-        <v>44835</v>
+        <v>44989</v>
       </c>
     </row>
     <row r="83" spans="1:3">
       <c r="A83" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B83">
-        <v>30</v>
+        <v>12.99</v>
       </c>
       <c r="C83" s="2">
-        <v>44744</v>
+        <v>44793</v>
       </c>
     </row>
     <row r="84" spans="1:3">
       <c r="A84" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B84">
-        <v>29</v>
+        <v>15.88</v>
       </c>
       <c r="C84" s="2">
-        <v>44744</v>
+        <v>44800</v>
       </c>
     </row>
     <row r="85" spans="1:3">
       <c r="A85" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B85">
-        <v>30.45</v>
+        <v>17.5</v>
       </c>
       <c r="C85" s="2">
-        <v>44870</v>
+        <v>44940</v>
       </c>
     </row>
     <row r="86" spans="1:3">
       <c r="A86" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B86">
-        <v>29.27</v>
+        <v>30</v>
       </c>
       <c r="C86" s="2">
         <v>44744</v>
@@ -1650,10 +1650,10 @@
     </row>
     <row r="87" spans="1:3">
       <c r="A87" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B87">
-        <v>32.3</v>
+        <v>31.5</v>
       </c>
       <c r="C87" s="2">
         <v>44835</v>
@@ -1661,10 +1661,10 @@
     </row>
     <row r="88" spans="1:3">
       <c r="A88" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B88">
-        <v>25.41</v>
+        <v>30</v>
       </c>
       <c r="C88" s="2">
         <v>44744</v>
@@ -1672,32 +1672,32 @@
     </row>
     <row r="89" spans="1:3">
       <c r="A89" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B89">
-        <v>26.73</v>
+        <v>29</v>
       </c>
       <c r="C89" s="2">
-        <v>44751</v>
+        <v>44744</v>
       </c>
     </row>
     <row r="90" spans="1:3">
       <c r="A90" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B90">
-        <v>29</v>
+        <v>30.45</v>
       </c>
       <c r="C90" s="2">
-        <v>44982</v>
+        <v>44870</v>
       </c>
     </row>
     <row r="91" spans="1:3">
       <c r="A91" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B91">
-        <v>21.58</v>
+        <v>29.27</v>
       </c>
       <c r="C91" s="2">
         <v>44744</v>
@@ -1705,54 +1705,54 @@
     </row>
     <row r="92" spans="1:3">
       <c r="A92" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B92">
-        <v>22.66</v>
+        <v>32.3</v>
       </c>
       <c r="C92" s="2">
-        <v>44751</v>
+        <v>44835</v>
       </c>
     </row>
     <row r="93" spans="1:3">
       <c r="A93" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B93">
-        <v>26.83</v>
+        <v>25.41</v>
       </c>
       <c r="C93" s="2">
-        <v>44814</v>
+        <v>44744</v>
       </c>
     </row>
     <row r="94" spans="1:3">
       <c r="A94" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B94">
-        <v>29</v>
+        <v>26.73</v>
       </c>
       <c r="C94" s="2">
-        <v>44982</v>
+        <v>44751</v>
       </c>
     </row>
     <row r="95" spans="1:3">
       <c r="A95" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B95">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="C95" s="2">
-        <v>44744</v>
+        <v>44982</v>
       </c>
     </row>
     <row r="96" spans="1:3">
       <c r="A96" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B96">
-        <v>28</v>
+        <v>21.58</v>
       </c>
       <c r="C96" s="2">
         <v>44744</v>
@@ -1760,54 +1760,54 @@
     </row>
     <row r="97" spans="1:3">
       <c r="A97" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B97">
-        <v>15.62</v>
+        <v>22.66</v>
       </c>
       <c r="C97" s="2">
-        <v>44744</v>
+        <v>44751</v>
       </c>
     </row>
     <row r="98" spans="1:3">
       <c r="A98" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B98">
-        <v>16.34</v>
+        <v>26.83</v>
       </c>
       <c r="C98" s="2">
-        <v>44751</v>
+        <v>44814</v>
       </c>
     </row>
     <row r="99" spans="1:3">
       <c r="A99" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B99">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C99" s="2">
-        <v>44859</v>
+        <v>44982</v>
       </c>
     </row>
     <row r="100" spans="1:3">
       <c r="A100" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B100">
-        <v>18.5</v>
+        <v>37</v>
       </c>
       <c r="C100" s="2">
-        <v>45003</v>
+        <v>44744</v>
       </c>
     </row>
     <row r="101" spans="1:3">
       <c r="A101" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B101">
-        <v>22.73</v>
+        <v>28</v>
       </c>
       <c r="C101" s="2">
         <v>44744</v>
@@ -1815,164 +1815,164 @@
     </row>
     <row r="102" spans="1:3">
       <c r="A102" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B102">
-        <v>23.77</v>
+        <v>15.62</v>
       </c>
       <c r="C102" s="2">
-        <v>44751</v>
+        <v>44744</v>
       </c>
     </row>
     <row r="103" spans="1:3">
       <c r="A103" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B103">
-        <v>24.59</v>
+        <v>16.34</v>
       </c>
       <c r="C103" s="2">
-        <v>44954</v>
+        <v>44751</v>
       </c>
     </row>
     <row r="104" spans="1:3">
       <c r="A104" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B104">
-        <v>18.76</v>
+        <v>30</v>
       </c>
       <c r="C104" s="2">
-        <v>44968</v>
+        <v>44859</v>
       </c>
     </row>
     <row r="105" spans="1:3">
       <c r="A105" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B105">
-        <v>26.73</v>
+        <v>364.64</v>
       </c>
       <c r="C105" s="2">
-        <v>45031</v>
+        <v>44996</v>
       </c>
     </row>
     <row r="106" spans="1:3">
       <c r="A106" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B106">
-        <v>23.77</v>
+        <v>18.5</v>
       </c>
       <c r="C106" s="2">
-        <v>45087</v>
+        <v>45003</v>
       </c>
     </row>
     <row r="107" spans="1:3">
       <c r="A107" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B107">
-        <v>37</v>
+        <v>22.73</v>
       </c>
       <c r="C107" s="2">
-        <v>45003</v>
+        <v>44744</v>
       </c>
     </row>
     <row r="108" spans="1:3">
       <c r="A108" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B108">
-        <v>15.62</v>
+        <v>23.77</v>
       </c>
       <c r="C108" s="2">
-        <v>44744</v>
+        <v>44751</v>
       </c>
     </row>
     <row r="109" spans="1:3">
       <c r="A109" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B109">
-        <v>16.34</v>
+        <v>196.72</v>
       </c>
       <c r="C109" s="2">
-        <v>44751</v>
+        <v>44947</v>
       </c>
     </row>
     <row r="110" spans="1:3">
       <c r="A110" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B110">
-        <v>18.5</v>
+        <v>380.32</v>
       </c>
       <c r="C110" s="2">
-        <v>45024</v>
+        <v>44947</v>
       </c>
     </row>
     <row r="111" spans="1:3">
       <c r="A111" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B111">
-        <v>15.62</v>
+        <v>24.59</v>
       </c>
       <c r="C111" s="2">
-        <v>44744</v>
+        <v>44954</v>
       </c>
     </row>
     <row r="112" spans="1:3">
       <c r="A112" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B112">
-        <v>23.77</v>
+        <v>18.76</v>
       </c>
       <c r="C112" s="2">
-        <v>44751</v>
+        <v>44968</v>
       </c>
     </row>
     <row r="113" spans="1:3">
       <c r="A113" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B113">
-        <v>24.59</v>
+        <v>26.73</v>
       </c>
       <c r="C113" s="2">
-        <v>44954</v>
+        <v>45031</v>
       </c>
     </row>
     <row r="114" spans="1:3">
       <c r="A114" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B114">
-        <v>32</v>
+        <v>23.77</v>
       </c>
       <c r="C114" s="2">
-        <v>44744</v>
+        <v>45087</v>
       </c>
     </row>
     <row r="115" spans="1:3">
       <c r="A115" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B115">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C115" s="2">
-        <v>44751</v>
+        <v>45003</v>
       </c>
     </row>
     <row r="116" spans="1:3">
       <c r="A116" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B116">
-        <v>30</v>
+        <v>15.62</v>
       </c>
       <c r="C116" s="2">
         <v>44744</v>
@@ -1980,142 +1980,142 @@
     </row>
     <row r="117" spans="1:3">
       <c r="A117" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B117">
-        <v>32</v>
+        <v>16.34</v>
       </c>
       <c r="C117" s="2">
-        <v>44835</v>
+        <v>44751</v>
       </c>
     </row>
     <row r="118" spans="1:3">
       <c r="A118" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B118">
-        <v>26.73</v>
+        <v>261.44</v>
       </c>
       <c r="C118" s="2">
-        <v>44954</v>
+        <v>45017</v>
       </c>
     </row>
     <row r="119" spans="1:3">
       <c r="A119" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B119">
-        <v>22.73</v>
+        <v>370</v>
       </c>
       <c r="C119" s="2">
-        <v>44744</v>
+        <v>45017</v>
       </c>
     </row>
     <row r="120" spans="1:3">
       <c r="A120" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B120">
-        <v>25.41</v>
+        <v>18.5</v>
       </c>
       <c r="C120" s="2">
-        <v>44744</v>
+        <v>45024</v>
       </c>
     </row>
     <row r="121" spans="1:3">
       <c r="A121" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B121">
-        <v>23.77</v>
+        <v>549.08</v>
       </c>
       <c r="C121" s="2">
-        <v>44751</v>
+        <v>45087</v>
       </c>
     </row>
     <row r="122" spans="1:3">
       <c r="A122" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B122">
-        <v>26.73</v>
+        <v>15.62</v>
       </c>
       <c r="C122" s="2">
-        <v>44751</v>
+        <v>44744</v>
       </c>
     </row>
     <row r="123" spans="1:3">
       <c r="A123" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B123">
-        <v>24.59</v>
+        <v>23.77</v>
       </c>
       <c r="C123" s="2">
-        <v>44828</v>
+        <v>44751</v>
       </c>
     </row>
     <row r="124" spans="1:3">
       <c r="A124" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B124">
-        <v>32</v>
+        <v>380.32</v>
       </c>
       <c r="C124" s="2">
-        <v>44744</v>
+        <v>44947</v>
       </c>
     </row>
     <row r="125" spans="1:3">
       <c r="A125" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B125">
-        <v>17.86</v>
+        <v>540.98</v>
       </c>
       <c r="C125" s="2">
-        <v>44744</v>
+        <v>44947</v>
       </c>
     </row>
     <row r="126" spans="1:3">
       <c r="A126" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B126">
-        <v>29.27</v>
+        <v>24.59</v>
       </c>
       <c r="C126" s="2">
-        <v>44744</v>
+        <v>44954</v>
       </c>
     </row>
     <row r="127" spans="1:3">
       <c r="A127" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B127">
-        <v>16.34</v>
+        <v>32</v>
       </c>
       <c r="C127" s="2">
-        <v>44751</v>
+        <v>44744</v>
       </c>
     </row>
     <row r="128" spans="1:3">
       <c r="A128" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B128">
-        <v>34.32</v>
+        <v>34</v>
       </c>
       <c r="C128" s="2">
-        <v>44835</v>
+        <v>44751</v>
       </c>
     </row>
     <row r="129" spans="1:3">
       <c r="A129" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B129">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C129" s="2">
         <v>44744</v>
@@ -2123,109 +2123,109 @@
     </row>
     <row r="130" spans="1:3">
       <c r="A130" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B130">
-        <v>26.73</v>
+        <v>32</v>
       </c>
       <c r="C130" s="2">
-        <v>44765</v>
+        <v>44835</v>
       </c>
     </row>
     <row r="131" spans="1:3">
       <c r="A131" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B131">
-        <v>24.83</v>
+        <v>26.73</v>
       </c>
       <c r="C131" s="2">
-        <v>44828</v>
+        <v>44954</v>
       </c>
     </row>
     <row r="132" spans="1:3">
       <c r="A132" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B132">
-        <v>25</v>
+        <v>22.73</v>
       </c>
       <c r="C132" s="2">
-        <v>44947</v>
+        <v>44744</v>
       </c>
     </row>
     <row r="133" spans="1:3">
       <c r="A133" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B133">
-        <v>30</v>
+        <v>25.41</v>
       </c>
       <c r="C133" s="2">
-        <v>45080</v>
+        <v>44744</v>
       </c>
     </row>
     <row r="134" spans="1:3">
       <c r="A134" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B134">
-        <v>36.59</v>
+        <v>23.77</v>
       </c>
       <c r="C134" s="2">
-        <v>44856</v>
+        <v>44751</v>
       </c>
     </row>
     <row r="135" spans="1:3">
       <c r="A135" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B135">
-        <v>23.77</v>
+        <v>26.73</v>
       </c>
       <c r="C135" s="2">
-        <v>44940</v>
+        <v>44751</v>
       </c>
     </row>
     <row r="136" spans="1:3">
       <c r="A136" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B136">
         <v>24.59</v>
       </c>
       <c r="C136" s="2">
-        <v>45024</v>
+        <v>44828</v>
       </c>
     </row>
     <row r="137" spans="1:3">
       <c r="A137" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B137">
-        <v>30.23</v>
+        <v>32</v>
       </c>
       <c r="C137" s="2">
-        <v>45031</v>
+        <v>44744</v>
       </c>
     </row>
     <row r="138" spans="1:3">
       <c r="A138" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B138">
-        <v>28.34</v>
+        <v>17.86</v>
       </c>
       <c r="C138" s="2">
-        <v>44786</v>
+        <v>44744</v>
       </c>
     </row>
     <row r="139" spans="1:3">
       <c r="A139" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B139">
-        <v>22.73</v>
+        <v>29.27</v>
       </c>
       <c r="C139" s="2">
         <v>44744</v>
@@ -2233,43 +2233,43 @@
     </row>
     <row r="140" spans="1:3">
       <c r="A140" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B140">
-        <v>40.49</v>
+        <v>16.34</v>
       </c>
       <c r="C140" s="2">
-        <v>44744</v>
+        <v>44751</v>
       </c>
     </row>
     <row r="141" spans="1:3">
       <c r="A141" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B141">
-        <v>23.77</v>
+        <v>34.32</v>
       </c>
       <c r="C141" s="2">
-        <v>44751</v>
+        <v>44835</v>
       </c>
     </row>
     <row r="142" spans="1:3">
       <c r="A142" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B142">
-        <v>50.47</v>
+        <v>28</v>
       </c>
       <c r="C142" s="2">
-        <v>44751</v>
+        <v>44744</v>
       </c>
     </row>
     <row r="143" spans="1:3">
       <c r="A143" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B143">
-        <v>12.99</v>
+        <v>26.73</v>
       </c>
       <c r="C143" s="2">
         <v>44765</v>
@@ -2277,164 +2277,164 @@
     </row>
     <row r="144" spans="1:3">
       <c r="A144" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B144">
-        <v>12.99</v>
+        <v>24.83</v>
       </c>
       <c r="C144" s="2">
-        <v>44940</v>
+        <v>44828</v>
       </c>
     </row>
     <row r="145" spans="1:3">
       <c r="A145" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B145">
-        <v>16.34</v>
+        <v>25</v>
       </c>
       <c r="C145" s="2">
-        <v>45038</v>
+        <v>44947</v>
       </c>
     </row>
     <row r="146" spans="1:3">
       <c r="A146" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B146">
-        <v>50.47</v>
+        <v>200</v>
       </c>
       <c r="C146" s="2">
-        <v>44933</v>
+        <v>45066</v>
       </c>
     </row>
     <row r="147" spans="1:3">
       <c r="A147" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B147">
-        <v>18.76</v>
+        <v>894.3</v>
       </c>
       <c r="C147" s="2">
-        <v>44961</v>
+        <v>45066</v>
       </c>
     </row>
     <row r="148" spans="1:3">
       <c r="A148" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B148">
-        <v>16.34</v>
+        <v>1132.3</v>
       </c>
       <c r="C148" s="2">
-        <v>44968</v>
+        <v>45073</v>
       </c>
     </row>
     <row r="149" spans="1:3">
       <c r="A149" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B149">
-        <v>55.52</v>
+        <v>30</v>
       </c>
       <c r="C149" s="2">
-        <v>45101</v>
+        <v>45080</v>
       </c>
     </row>
     <row r="150" spans="1:3">
       <c r="A150" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B150">
-        <v>41</v>
+        <v>36.59</v>
       </c>
       <c r="C150" s="2">
-        <v>44772</v>
+        <v>44856</v>
       </c>
     </row>
     <row r="151" spans="1:3">
       <c r="A151" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="B151">
-        <v>30</v>
+        <v>1390.41</v>
       </c>
       <c r="C151" s="2">
-        <v>44744</v>
+        <v>45080</v>
       </c>
     </row>
     <row r="152" spans="1:3">
       <c r="A152" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="B152">
-        <v>15.11</v>
+        <v>23.77</v>
       </c>
       <c r="C152" s="2">
-        <v>44744</v>
+        <v>44940</v>
       </c>
     </row>
     <row r="153" spans="1:3">
       <c r="A153" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="B153">
-        <v>32</v>
+        <v>380.32</v>
       </c>
       <c r="C153" s="2">
-        <v>44744</v>
+        <v>45017</v>
       </c>
     </row>
     <row r="154" spans="1:3">
       <c r="A154" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="B154">
-        <v>16.34</v>
+        <v>540.98</v>
       </c>
       <c r="C154" s="2">
-        <v>44751</v>
+        <v>45017</v>
       </c>
     </row>
     <row r="155" spans="1:3">
       <c r="A155" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="B155">
-        <v>15.88</v>
+        <v>24.59</v>
       </c>
       <c r="C155" s="2">
-        <v>45017</v>
+        <v>45024</v>
       </c>
     </row>
     <row r="156" spans="1:3">
       <c r="A156" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="B156">
-        <v>18.76</v>
+        <v>30.23</v>
       </c>
       <c r="C156" s="2">
-        <v>45024</v>
+        <v>45031</v>
       </c>
     </row>
     <row r="157" spans="1:3">
       <c r="A157" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="B157">
-        <v>15.62</v>
+        <v>28.34</v>
       </c>
       <c r="C157" s="2">
-        <v>44744</v>
+        <v>44786</v>
       </c>
     </row>
     <row r="158" spans="1:3">
       <c r="A158" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B158">
-        <v>30</v>
+        <v>22.73</v>
       </c>
       <c r="C158" s="2">
         <v>44744</v>
@@ -2442,54 +2442,54 @@
     </row>
     <row r="159" spans="1:3">
       <c r="A159" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B159">
-        <v>16.34</v>
+        <v>40.49</v>
       </c>
       <c r="C159" s="2">
-        <v>44751</v>
+        <v>44744</v>
       </c>
     </row>
     <row r="160" spans="1:3">
       <c r="A160" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B160">
-        <v>31.5</v>
+        <v>23.77</v>
       </c>
       <c r="C160" s="2">
-        <v>44835</v>
+        <v>44751</v>
       </c>
     </row>
     <row r="161" spans="1:3">
       <c r="A161" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B161">
-        <v>18.5</v>
+        <v>50.47</v>
       </c>
       <c r="C161" s="2">
-        <v>45024</v>
+        <v>44751</v>
       </c>
     </row>
     <row r="162" spans="1:3">
       <c r="A162" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B162">
-        <v>26.73</v>
+        <v>12.99</v>
       </c>
       <c r="C162" s="2">
-        <v>44758</v>
+        <v>44765</v>
       </c>
     </row>
     <row r="163" spans="1:3">
       <c r="A163" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B163">
-        <v>60.56</v>
+        <v>12.99</v>
       </c>
       <c r="C163" s="2">
         <v>44940</v>
@@ -2497,164 +2497,164 @@
     </row>
     <row r="164" spans="1:3">
       <c r="A164" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B164">
-        <v>30</v>
+        <v>16.34</v>
       </c>
       <c r="C164" s="2">
-        <v>44968</v>
+        <v>45038</v>
       </c>
     </row>
     <row r="165" spans="1:3">
       <c r="A165" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B165">
-        <v>22.73</v>
+        <v>50.47</v>
       </c>
       <c r="C165" s="2">
-        <v>44744</v>
+        <v>44933</v>
       </c>
     </row>
     <row r="166" spans="1:3">
       <c r="A166" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B166">
-        <v>34</v>
+        <v>18.76</v>
       </c>
       <c r="C166" s="2">
-        <v>44744</v>
+        <v>44961</v>
       </c>
     </row>
     <row r="167" spans="1:3">
       <c r="A167" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B167">
-        <v>54.66</v>
+        <v>16.34</v>
       </c>
       <c r="C167" s="2">
-        <v>44744</v>
+        <v>44968</v>
       </c>
     </row>
     <row r="168" spans="1:3">
       <c r="A168" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B168">
-        <v>70.66</v>
+        <v>55.52</v>
       </c>
       <c r="C168" s="2">
-        <v>44744</v>
+        <v>45101</v>
       </c>
     </row>
     <row r="169" spans="1:3">
       <c r="A169" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B169">
-        <v>23.77</v>
+        <v>41</v>
       </c>
       <c r="C169" s="2">
-        <v>44751</v>
+        <v>44772</v>
       </c>
     </row>
     <row r="170" spans="1:3">
       <c r="A170" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B170">
-        <v>60.56</v>
+        <v>30</v>
       </c>
       <c r="C170" s="2">
-        <v>44835</v>
+        <v>44744</v>
       </c>
     </row>
     <row r="171" spans="1:3">
       <c r="A171" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B171">
-        <v>70.66</v>
+        <v>15.11</v>
       </c>
       <c r="C171" s="2">
-        <v>44933</v>
+        <v>44744</v>
       </c>
     </row>
     <row r="172" spans="1:3">
       <c r="A172" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B172">
-        <v>15.88</v>
+        <v>32</v>
       </c>
       <c r="C172" s="2">
-        <v>44982</v>
+        <v>44744</v>
       </c>
     </row>
     <row r="173" spans="1:3">
       <c r="A173" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B173">
         <v>16.34</v>
       </c>
       <c r="C173" s="2">
-        <v>45087</v>
+        <v>44751</v>
       </c>
     </row>
     <row r="174" spans="1:3">
       <c r="A174" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B174">
-        <v>34</v>
+        <v>477.95</v>
       </c>
       <c r="C174" s="2">
-        <v>44744</v>
+        <v>45010</v>
       </c>
     </row>
     <row r="175" spans="1:3">
       <c r="A175" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B175">
-        <v>42.9</v>
+        <v>15.88</v>
       </c>
       <c r="C175" s="2">
-        <v>44744</v>
+        <v>45017</v>
       </c>
     </row>
     <row r="176" spans="1:3">
       <c r="A176" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B176">
-        <v>37</v>
+        <v>18.76</v>
       </c>
       <c r="C176" s="2">
-        <v>44828</v>
+        <v>45024</v>
       </c>
     </row>
     <row r="177" spans="1:3">
       <c r="A177" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B177">
-        <v>42.9</v>
+        <v>-972.8</v>
       </c>
       <c r="C177" s="2">
-        <v>44744</v>
+        <v>45045</v>
       </c>
     </row>
     <row r="178" spans="1:3">
       <c r="A178" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B178">
-        <v>35.33</v>
+        <v>15.62</v>
       </c>
       <c r="C178" s="2">
         <v>44744</v>
@@ -2662,120 +2662,120 @@
     </row>
     <row r="179" spans="1:3">
       <c r="A179" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B179">
-        <v>37.85</v>
+        <v>30</v>
       </c>
       <c r="C179" s="2">
-        <v>44947</v>
+        <v>44744</v>
       </c>
     </row>
     <row r="180" spans="1:3">
       <c r="A180" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B180">
-        <v>39.11</v>
+        <v>16.34</v>
       </c>
       <c r="C180" s="2">
-        <v>45059</v>
+        <v>44751</v>
       </c>
     </row>
     <row r="181" spans="1:3">
       <c r="A181" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="B181">
-        <v>17.86</v>
+        <v>31.5</v>
       </c>
       <c r="C181" s="2">
-        <v>44744</v>
+        <v>44835</v>
       </c>
     </row>
     <row r="182" spans="1:3">
       <c r="A182" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="B182">
-        <v>22.73</v>
+        <v>130.72</v>
       </c>
       <c r="C182" s="2">
-        <v>44744</v>
+        <v>45017</v>
       </c>
     </row>
     <row r="183" spans="1:3">
       <c r="A183" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="B183">
-        <v>18.76</v>
+        <v>407</v>
       </c>
       <c r="C183" s="2">
-        <v>44751</v>
+        <v>45017</v>
       </c>
     </row>
     <row r="184" spans="1:3">
       <c r="A184" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="B184">
-        <v>23.77</v>
+        <v>18.5</v>
       </c>
       <c r="C184" s="2">
-        <v>44751</v>
+        <v>45024</v>
       </c>
     </row>
     <row r="185" spans="1:3">
       <c r="A185" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B185">
-        <v>16.34</v>
+        <v>26.73</v>
       </c>
       <c r="C185" s="2">
-        <v>44835</v>
+        <v>44758</v>
       </c>
     </row>
     <row r="186" spans="1:3">
       <c r="A186" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B186">
-        <v>14.23</v>
+        <v>60.56</v>
       </c>
       <c r="C186" s="2">
-        <v>44898</v>
+        <v>44940</v>
       </c>
     </row>
     <row r="187" spans="1:3">
       <c r="A187" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B187">
-        <v>17.08</v>
+        <v>30</v>
       </c>
       <c r="C187" s="2">
-        <v>44905</v>
+        <v>44968</v>
       </c>
     </row>
     <row r="188" spans="1:3">
       <c r="A188" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B188">
-        <v>24.59</v>
+        <v>22.73</v>
       </c>
       <c r="C188" s="2">
-        <v>45024</v>
+        <v>44744</v>
       </c>
     </row>
     <row r="189" spans="1:3">
       <c r="A189" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B189">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C189" s="2">
         <v>44744</v>
@@ -2783,98 +2783,98 @@
     </row>
     <row r="190" spans="1:3">
       <c r="A190" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B190">
-        <v>26.73</v>
+        <v>54.66</v>
       </c>
       <c r="C190" s="2">
-        <v>44765</v>
+        <v>44744</v>
       </c>
     </row>
     <row r="191" spans="1:3">
       <c r="A191" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B191">
-        <v>35</v>
+        <v>70.66</v>
       </c>
       <c r="C191" s="2">
-        <v>44835</v>
+        <v>44744</v>
       </c>
     </row>
     <row r="192" spans="1:3">
       <c r="A192" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B192">
         <v>23.77</v>
       </c>
       <c r="C192" s="2">
-        <v>44968</v>
+        <v>44751</v>
       </c>
     </row>
     <row r="193" spans="1:3">
       <c r="A193" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="B193">
-        <v>35</v>
+        <v>60.56</v>
       </c>
       <c r="C193" s="2">
-        <v>44933</v>
+        <v>44835</v>
       </c>
     </row>
     <row r="194" spans="1:3">
       <c r="A194" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B194">
-        <v>26.73</v>
+        <v>70.66</v>
       </c>
       <c r="C194" s="2">
-        <v>44968</v>
+        <v>44933</v>
       </c>
     </row>
     <row r="195" spans="1:3">
       <c r="A195" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B195">
-        <v>23.77</v>
+        <v>15.88</v>
       </c>
       <c r="C195" s="2">
-        <v>45087</v>
+        <v>44982</v>
       </c>
     </row>
     <row r="196" spans="1:3">
       <c r="A196" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="B196">
-        <v>30</v>
+        <v>16.34</v>
       </c>
       <c r="C196" s="2">
-        <v>44744</v>
+        <v>45087</v>
       </c>
     </row>
     <row r="197" spans="1:3">
       <c r="A197" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B197">
-        <v>31.5</v>
+        <v>34</v>
       </c>
       <c r="C197" s="2">
-        <v>44835</v>
+        <v>44744</v>
       </c>
     </row>
     <row r="198" spans="1:3">
       <c r="A198" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="B198">
-        <v>17.86</v>
+        <v>42.9</v>
       </c>
       <c r="C198" s="2">
         <v>44744</v>
@@ -2882,76 +2882,76 @@
     </row>
     <row r="199" spans="1:3">
       <c r="A199" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="B199">
-        <v>28.5</v>
+        <v>37</v>
       </c>
       <c r="C199" s="2">
-        <v>44744</v>
+        <v>44828</v>
       </c>
     </row>
     <row r="200" spans="1:3">
       <c r="A200" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B200">
-        <v>18.76</v>
+        <v>42.9</v>
       </c>
       <c r="C200" s="2">
-        <v>44751</v>
+        <v>44744</v>
       </c>
     </row>
     <row r="201" spans="1:3">
       <c r="A201" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B201">
-        <v>22.66</v>
+        <v>1630.14</v>
       </c>
       <c r="C201" s="2">
-        <v>44779</v>
+        <v>44996</v>
       </c>
     </row>
     <row r="202" spans="1:3">
       <c r="A202" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B202">
-        <v>16.34</v>
+        <v>35.33</v>
       </c>
       <c r="C202" s="2">
-        <v>44982</v>
+        <v>44744</v>
       </c>
     </row>
     <row r="203" spans="1:3">
       <c r="A203" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B203">
-        <v>26.73</v>
+        <v>37.85</v>
       </c>
       <c r="C203" s="2">
-        <v>44940</v>
+        <v>44947</v>
       </c>
     </row>
     <row r="204" spans="1:3">
       <c r="A204" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B204">
-        <v>23.77</v>
+        <v>39.11</v>
       </c>
       <c r="C204" s="2">
-        <v>45038</v>
+        <v>45059</v>
       </c>
     </row>
     <row r="205" spans="1:3">
       <c r="A205" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B205">
-        <v>28</v>
+        <v>17.86</v>
       </c>
       <c r="C205" s="2">
         <v>44744</v>
@@ -2959,109 +2959,109 @@
     </row>
     <row r="206" spans="1:3">
       <c r="A206" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B206">
-        <v>30</v>
+        <v>22.73</v>
       </c>
       <c r="C206" s="2">
-        <v>44856</v>
+        <v>44744</v>
       </c>
     </row>
     <row r="207" spans="1:3">
       <c r="A207" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B207">
-        <v>35</v>
+        <v>18.76</v>
       </c>
       <c r="C207" s="2">
-        <v>45087</v>
+        <v>44751</v>
       </c>
     </row>
     <row r="208" spans="1:3">
       <c r="A208" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="B208">
-        <v>37.85</v>
+        <v>23.77</v>
       </c>
       <c r="C208" s="2">
-        <v>44744</v>
+        <v>44751</v>
       </c>
     </row>
     <row r="209" spans="1:3">
       <c r="A209" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="B209">
-        <v>42.9</v>
+        <v>16.34</v>
       </c>
       <c r="C209" s="2">
-        <v>45101</v>
+        <v>44835</v>
       </c>
     </row>
     <row r="210" spans="1:3">
       <c r="A210" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="B210">
-        <v>32</v>
+        <v>14.23</v>
       </c>
       <c r="C210" s="2">
-        <v>44744</v>
+        <v>44898</v>
       </c>
     </row>
     <row r="211" spans="1:3">
       <c r="A211" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="B211">
-        <v>26.73</v>
+        <v>17.08</v>
       </c>
       <c r="C211" s="2">
-        <v>44800</v>
+        <v>44905</v>
       </c>
     </row>
     <row r="212" spans="1:3">
       <c r="A212" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="B212">
-        <v>24.59</v>
+        <v>380.32</v>
       </c>
       <c r="C212" s="2">
-        <v>44828</v>
+        <v>45017</v>
       </c>
     </row>
     <row r="213" spans="1:3">
       <c r="A213" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="B213">
-        <v>31</v>
+        <v>540.98</v>
       </c>
       <c r="C213" s="2">
-        <v>44940</v>
+        <v>45017</v>
       </c>
     </row>
     <row r="214" spans="1:3">
       <c r="A214" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="B214">
-        <v>22.66</v>
+        <v>24.59</v>
       </c>
       <c r="C214" s="2">
-        <v>45073</v>
+        <v>45024</v>
       </c>
     </row>
     <row r="215" spans="1:3">
       <c r="A215" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="B215">
-        <v>17.86</v>
+        <v>33</v>
       </c>
       <c r="C215" s="2">
         <v>44744</v>
@@ -3069,76 +3069,76 @@
     </row>
     <row r="216" spans="1:3">
       <c r="A216" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="B216">
-        <v>18.76</v>
+        <v>26.73</v>
       </c>
       <c r="C216" s="2">
-        <v>44751</v>
+        <v>44765</v>
       </c>
     </row>
     <row r="217" spans="1:3">
       <c r="A217" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="B217">
-        <v>22.66</v>
+        <v>35</v>
       </c>
       <c r="C217" s="2">
-        <v>44779</v>
+        <v>44835</v>
       </c>
     </row>
     <row r="218" spans="1:3">
       <c r="A218" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="B218">
-        <v>26</v>
+        <v>23.77</v>
       </c>
       <c r="C218" s="2">
-        <v>44835</v>
+        <v>44968</v>
       </c>
     </row>
     <row r="219" spans="1:3">
       <c r="A219" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="B219">
-        <v>50.61</v>
+        <v>35</v>
       </c>
       <c r="C219" s="2">
-        <v>44744</v>
+        <v>44933</v>
       </c>
     </row>
     <row r="220" spans="1:3">
       <c r="A220" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="B220">
-        <v>60.56</v>
+        <v>26.73</v>
       </c>
       <c r="C220" s="2">
-        <v>44835</v>
+        <v>44968</v>
       </c>
     </row>
     <row r="221" spans="1:3">
       <c r="A221" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="B221">
-        <v>55.52</v>
+        <v>23.77</v>
       </c>
       <c r="C221" s="2">
-        <v>44744</v>
+        <v>45087</v>
       </c>
     </row>
     <row r="222" spans="1:3">
       <c r="A222" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="B222">
-        <v>17.86</v>
+        <v>30</v>
       </c>
       <c r="C222" s="2">
         <v>44744</v>
@@ -3146,131 +3146,131 @@
     </row>
     <row r="223" spans="1:3">
       <c r="A223" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="B223">
-        <v>32</v>
+        <v>31.5</v>
       </c>
       <c r="C223" s="2">
-        <v>44744</v>
+        <v>44835</v>
       </c>
     </row>
     <row r="224" spans="1:3">
       <c r="A224" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="B224">
-        <v>18.76</v>
+        <v>17.86</v>
       </c>
       <c r="C224" s="2">
-        <v>44751</v>
+        <v>44744</v>
       </c>
     </row>
     <row r="225" spans="1:3">
       <c r="A225" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="B225">
-        <v>16.34</v>
+        <v>28.5</v>
       </c>
       <c r="C225" s="2">
-        <v>44835</v>
+        <v>44744</v>
       </c>
     </row>
     <row r="226" spans="1:3">
       <c r="A226" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="B226">
-        <v>15.62</v>
+        <v>18.76</v>
       </c>
       <c r="C226" s="2">
-        <v>44744</v>
+        <v>44751</v>
       </c>
     </row>
     <row r="227" spans="1:3">
       <c r="A227" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="B227">
-        <v>16.34</v>
+        <v>22.66</v>
       </c>
       <c r="C227" s="2">
-        <v>44751</v>
+        <v>44779</v>
       </c>
     </row>
     <row r="228" spans="1:3">
       <c r="A228" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="B228">
-        <v>23.77</v>
+        <v>16.34</v>
       </c>
       <c r="C228" s="2">
-        <v>44821</v>
+        <v>44982</v>
       </c>
     </row>
     <row r="229" spans="1:3">
       <c r="A229" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="B229">
-        <v>24.59</v>
+        <v>26.73</v>
       </c>
       <c r="C229" s="2">
-        <v>45003</v>
+        <v>44940</v>
       </c>
     </row>
     <row r="230" spans="1:3">
       <c r="A230" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="B230">
-        <v>25.41</v>
+        <v>23.77</v>
       </c>
       <c r="C230" s="2">
-        <v>44744</v>
+        <v>45038</v>
       </c>
     </row>
     <row r="231" spans="1:3">
       <c r="A231" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="B231">
-        <v>26.73</v>
+        <v>28</v>
       </c>
       <c r="C231" s="2">
-        <v>44751</v>
+        <v>44744</v>
       </c>
     </row>
     <row r="232" spans="1:3">
       <c r="A232" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="B232">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C232" s="2">
-        <v>45087</v>
+        <v>44856</v>
       </c>
     </row>
     <row r="233" spans="1:3">
       <c r="A233" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="B233">
-        <v>30.95</v>
+        <v>35</v>
       </c>
       <c r="C233" s="2">
-        <v>44751</v>
+        <v>45087</v>
       </c>
     </row>
     <row r="234" spans="1:3">
       <c r="A234" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="B234">
-        <v>25.41</v>
+        <v>37.85</v>
       </c>
       <c r="C234" s="2">
         <v>44744</v>
@@ -3278,21 +3278,21 @@
     </row>
     <row r="235" spans="1:3">
       <c r="A235" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="B235">
-        <v>26.73</v>
+        <v>42.9</v>
       </c>
       <c r="C235" s="2">
-        <v>44751</v>
+        <v>45101</v>
       </c>
     </row>
     <row r="236" spans="1:3">
       <c r="A236" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="B236">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C236" s="2">
         <v>44744</v>
@@ -3300,76 +3300,76 @@
     </row>
     <row r="237" spans="1:3">
       <c r="A237" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="B237">
-        <v>28.08</v>
+        <v>26.73</v>
       </c>
       <c r="C237" s="2">
-        <v>44744</v>
+        <v>44800</v>
       </c>
     </row>
     <row r="238" spans="1:3">
       <c r="A238" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="B238">
-        <v>29.39</v>
+        <v>24.59</v>
       </c>
       <c r="C238" s="2">
-        <v>44758</v>
+        <v>44828</v>
       </c>
     </row>
     <row r="239" spans="1:3">
       <c r="A239" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="B239">
-        <v>15.62</v>
+        <v>31</v>
       </c>
       <c r="C239" s="2">
-        <v>44744</v>
+        <v>44940</v>
       </c>
     </row>
     <row r="240" spans="1:3">
       <c r="A240" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="B240">
-        <v>16.34</v>
+        <v>22.66</v>
       </c>
       <c r="C240" s="2">
-        <v>44751</v>
+        <v>45073</v>
       </c>
     </row>
     <row r="241" spans="1:3">
       <c r="A241" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="B241">
-        <v>18.5</v>
+        <v>17.86</v>
       </c>
       <c r="C241" s="2">
-        <v>45024</v>
+        <v>44744</v>
       </c>
     </row>
     <row r="242" spans="1:3">
       <c r="A242" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="B242">
-        <v>32</v>
+        <v>18.76</v>
       </c>
       <c r="C242" s="2">
-        <v>44744</v>
+        <v>44751</v>
       </c>
     </row>
     <row r="243" spans="1:3">
       <c r="A243" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="B243">
-        <v>34</v>
+        <v>22.66</v>
       </c>
       <c r="C243" s="2">
         <v>44779</v>
@@ -3377,21 +3377,21 @@
     </row>
     <row r="244" spans="1:3">
       <c r="A244" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="B244">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="C244" s="2">
-        <v>44772</v>
+        <v>44835</v>
       </c>
     </row>
     <row r="245" spans="1:3">
       <c r="A245" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="B245">
-        <v>24.32</v>
+        <v>50.61</v>
       </c>
       <c r="C245" s="2">
         <v>44744</v>
@@ -3399,32 +3399,32 @@
     </row>
     <row r="246" spans="1:3">
       <c r="A246" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="B246">
-        <v>25.05</v>
+        <v>60.56</v>
       </c>
       <c r="C246" s="2">
-        <v>44751</v>
+        <v>44835</v>
       </c>
     </row>
     <row r="247" spans="1:3">
       <c r="A247" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="B247">
-        <v>31</v>
+        <v>55.52</v>
       </c>
       <c r="C247" s="2">
-        <v>44863</v>
+        <v>44744</v>
       </c>
     </row>
     <row r="248" spans="1:3">
       <c r="A248" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="B248">
-        <v>25.41</v>
+        <v>17.86</v>
       </c>
       <c r="C248" s="2">
         <v>44744</v>
@@ -3432,43 +3432,43 @@
     </row>
     <row r="249" spans="1:3">
       <c r="A249" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="B249">
-        <v>23.77</v>
+        <v>32</v>
       </c>
       <c r="C249" s="2">
-        <v>44751</v>
+        <v>44744</v>
       </c>
     </row>
     <row r="250" spans="1:3">
       <c r="A250" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="B250">
-        <v>26.73</v>
+        <v>18.76</v>
       </c>
       <c r="C250" s="2">
-        <v>44982</v>
+        <v>44751</v>
       </c>
     </row>
     <row r="251" spans="1:3">
       <c r="A251" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="B251">
-        <v>28.5</v>
+        <v>16.34</v>
       </c>
       <c r="C251" s="2">
-        <v>45059</v>
+        <v>44835</v>
       </c>
     </row>
     <row r="252" spans="1:3">
       <c r="A252" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="B252">
-        <v>25.41</v>
+        <v>15.62</v>
       </c>
       <c r="C252" s="2">
         <v>44744</v>
@@ -3476,10 +3476,10 @@
     </row>
     <row r="253" spans="1:3">
       <c r="A253" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="B253">
-        <v>26.73</v>
+        <v>16.34</v>
       </c>
       <c r="C253" s="2">
         <v>44751</v>
@@ -3487,144 +3487,507 @@
     </row>
     <row r="254" spans="1:3">
       <c r="A254" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="B254">
-        <v>28</v>
+        <v>23.77</v>
       </c>
       <c r="C254" s="2">
-        <v>44744</v>
+        <v>44821</v>
       </c>
     </row>
     <row r="255" spans="1:3">
       <c r="A255" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="B255">
-        <v>40.49</v>
+        <v>350.41</v>
       </c>
       <c r="C255" s="2">
-        <v>44744</v>
+        <v>44996</v>
       </c>
     </row>
     <row r="256" spans="1:3">
       <c r="A256" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="B256">
-        <v>52.99</v>
+        <v>361.3</v>
       </c>
       <c r="C256" s="2">
-        <v>44835</v>
+        <v>44996</v>
       </c>
     </row>
     <row r="257" spans="1:3">
       <c r="A257" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
       <c r="B257">
-        <v>31.29</v>
+        <v>24.59</v>
       </c>
       <c r="C257" s="2">
-        <v>45024</v>
+        <v>45003</v>
       </c>
     </row>
     <row r="258" spans="1:3">
       <c r="A258" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="B258">
-        <v>25.03</v>
+        <v>25.41</v>
       </c>
       <c r="C258" s="2">
-        <v>45066</v>
+        <v>44744</v>
       </c>
     </row>
     <row r="259" spans="1:3">
       <c r="A259" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="B259">
-        <v>45.42</v>
+        <v>26.73</v>
       </c>
       <c r="C259" s="2">
-        <v>45038</v>
+        <v>44751</v>
       </c>
     </row>
     <row r="260" spans="1:3">
       <c r="A260" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
       <c r="B260">
-        <v>26.83</v>
+        <v>35</v>
       </c>
       <c r="C260" s="2">
-        <v>44954</v>
+        <v>45087</v>
       </c>
     </row>
     <row r="261" spans="1:3">
       <c r="A261" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
       <c r="B261">
-        <v>26</v>
+        <v>30.95</v>
       </c>
       <c r="C261" s="2">
-        <v>44744</v>
+        <v>44751</v>
       </c>
     </row>
     <row r="262" spans="1:3">
       <c r="A262" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="B262">
-        <v>26.73</v>
+        <v>25.41</v>
       </c>
       <c r="C262" s="2">
-        <v>44751</v>
+        <v>44744</v>
       </c>
     </row>
     <row r="263" spans="1:3">
       <c r="A263" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="B263">
-        <v>24.06</v>
+        <v>26.73</v>
       </c>
       <c r="C263" s="2">
-        <v>44744</v>
+        <v>44751</v>
       </c>
     </row>
     <row r="264" spans="1:3">
       <c r="A264" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="B264">
-        <v>24.61</v>
+        <v>38</v>
       </c>
       <c r="C264" s="2">
-        <v>44751</v>
+        <v>44744</v>
       </c>
     </row>
     <row r="265" spans="1:3">
       <c r="A265" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="B265">
-        <v>24.83</v>
+        <v>28.08</v>
       </c>
       <c r="C265" s="2">
-        <v>44814</v>
+        <v>44744</v>
       </c>
     </row>
     <row r="266" spans="1:3">
       <c r="A266" t="s">
+        <v>92</v>
+      </c>
+      <c r="B266">
+        <v>29.39</v>
+      </c>
+      <c r="C266" s="2">
+        <v>44758</v>
+      </c>
+    </row>
+    <row r="267" spans="1:3">
+      <c r="A267" t="s">
+        <v>93</v>
+      </c>
+      <c r="B267">
+        <v>15.62</v>
+      </c>
+      <c r="C267" s="2">
+        <v>44744</v>
+      </c>
+    </row>
+    <row r="268" spans="1:3">
+      <c r="A268" t="s">
+        <v>93</v>
+      </c>
+      <c r="B268">
+        <v>16.34</v>
+      </c>
+      <c r="C268" s="2">
+        <v>44751</v>
+      </c>
+    </row>
+    <row r="269" spans="1:3">
+      <c r="A269" t="s">
+        <v>93</v>
+      </c>
+      <c r="B269">
+        <v>130.72</v>
+      </c>
+      <c r="C269" s="2">
+        <v>45017</v>
+      </c>
+    </row>
+    <row r="270" spans="1:3">
+      <c r="A270" t="s">
+        <v>93</v>
+      </c>
+      <c r="B270">
+        <v>407</v>
+      </c>
+      <c r="C270" s="2">
+        <v>45017</v>
+      </c>
+    </row>
+    <row r="271" spans="1:3">
+      <c r="A271" t="s">
+        <v>93</v>
+      </c>
+      <c r="B271">
+        <v>18.5</v>
+      </c>
+      <c r="C271" s="2">
+        <v>45024</v>
+      </c>
+    </row>
+    <row r="272" spans="1:3">
+      <c r="A272" t="s">
+        <v>94</v>
+      </c>
+      <c r="B272">
+        <v>32</v>
+      </c>
+      <c r="C272" s="2">
+        <v>44744</v>
+      </c>
+    </row>
+    <row r="273" spans="1:3">
+      <c r="A273" t="s">
+        <v>94</v>
+      </c>
+      <c r="B273">
+        <v>34</v>
+      </c>
+      <c r="C273" s="2">
+        <v>44779</v>
+      </c>
+    </row>
+    <row r="274" spans="1:3">
+      <c r="A274" t="s">
+        <v>95</v>
+      </c>
+      <c r="B274">
+        <v>35</v>
+      </c>
+      <c r="C274" s="2">
+        <v>44772</v>
+      </c>
+    </row>
+    <row r="275" spans="1:3">
+      <c r="A275" t="s">
+        <v>96</v>
+      </c>
+      <c r="B275">
+        <v>24.32</v>
+      </c>
+      <c r="C275" s="2">
+        <v>44744</v>
+      </c>
+    </row>
+    <row r="276" spans="1:3">
+      <c r="A276" t="s">
+        <v>96</v>
+      </c>
+      <c r="B276">
+        <v>25.05</v>
+      </c>
+      <c r="C276" s="2">
+        <v>44751</v>
+      </c>
+    </row>
+    <row r="277" spans="1:3">
+      <c r="A277" t="s">
+        <v>96</v>
+      </c>
+      <c r="B277">
+        <v>31</v>
+      </c>
+      <c r="C277" s="2">
+        <v>44863</v>
+      </c>
+    </row>
+    <row r="278" spans="1:3">
+      <c r="A278" t="s">
+        <v>96</v>
+      </c>
+      <c r="B278">
+        <v>1085.62</v>
+      </c>
+      <c r="C278" s="2">
+        <v>44961</v>
+      </c>
+    </row>
+    <row r="279" spans="1:3">
+      <c r="A279" t="s">
+        <v>97</v>
+      </c>
+      <c r="B279">
+        <v>25.41</v>
+      </c>
+      <c r="C279" s="2">
+        <v>44744</v>
+      </c>
+    </row>
+    <row r="280" spans="1:3">
+      <c r="A280" t="s">
+        <v>97</v>
+      </c>
+      <c r="B280">
+        <v>23.77</v>
+      </c>
+      <c r="C280" s="2">
+        <v>44751</v>
+      </c>
+    </row>
+    <row r="281" spans="1:3">
+      <c r="A281" t="s">
+        <v>98</v>
+      </c>
+      <c r="B281">
+        <v>26.73</v>
+      </c>
+      <c r="C281" s="2">
+        <v>44982</v>
+      </c>
+    </row>
+    <row r="282" spans="1:3">
+      <c r="A282" t="s">
+        <v>98</v>
+      </c>
+      <c r="B282">
+        <v>28.5</v>
+      </c>
+      <c r="C282" s="2">
+        <v>45059</v>
+      </c>
+    </row>
+    <row r="283" spans="1:3">
+      <c r="A283" t="s">
+        <v>99</v>
+      </c>
+      <c r="B283">
+        <v>25.41</v>
+      </c>
+      <c r="C283" s="2">
+        <v>44744</v>
+      </c>
+    </row>
+    <row r="284" spans="1:3">
+      <c r="A284" t="s">
+        <v>99</v>
+      </c>
+      <c r="B284">
+        <v>26.73</v>
+      </c>
+      <c r="C284" s="2">
+        <v>44751</v>
+      </c>
+    </row>
+    <row r="285" spans="1:3">
+      <c r="A285" t="s">
+        <v>100</v>
+      </c>
+      <c r="B285">
+        <v>28</v>
+      </c>
+      <c r="C285" s="2">
+        <v>44744</v>
+      </c>
+    </row>
+    <row r="286" spans="1:3">
+      <c r="A286" t="s">
+        <v>101</v>
+      </c>
+      <c r="B286">
+        <v>40.49</v>
+      </c>
+      <c r="C286" s="2">
+        <v>44744</v>
+      </c>
+    </row>
+    <row r="287" spans="1:3">
+      <c r="A287" t="s">
+        <v>101</v>
+      </c>
+      <c r="B287">
+        <v>52.99</v>
+      </c>
+      <c r="C287" s="2">
+        <v>44835</v>
+      </c>
+    </row>
+    <row r="288" spans="1:3">
+      <c r="A288" t="s">
+        <v>102</v>
+      </c>
+      <c r="B288">
+        <v>31.29</v>
+      </c>
+      <c r="C288" s="2">
+        <v>45024</v>
+      </c>
+    </row>
+    <row r="289" spans="1:3">
+      <c r="A289" t="s">
+        <v>102</v>
+      </c>
+      <c r="B289">
+        <v>25.03</v>
+      </c>
+      <c r="C289" s="2">
+        <v>45066</v>
+      </c>
+    </row>
+    <row r="290" spans="1:3">
+      <c r="A290" t="s">
+        <v>102</v>
+      </c>
+      <c r="B290">
+        <v>156.5</v>
+      </c>
+      <c r="C290" s="2">
+        <v>45073</v>
+      </c>
+    </row>
+    <row r="291" spans="1:3">
+      <c r="A291" t="s">
+        <v>102</v>
+      </c>
+      <c r="B291">
+        <v>860.48</v>
+      </c>
+      <c r="C291" s="2">
+        <v>45073</v>
+      </c>
+    </row>
+    <row r="292" spans="1:3">
+      <c r="A292" t="s">
+        <v>103</v>
+      </c>
+      <c r="B292">
+        <v>45.42</v>
+      </c>
+      <c r="C292" s="2">
+        <v>45038</v>
+      </c>
+    </row>
+    <row r="293" spans="1:3">
+      <c r="A293" t="s">
+        <v>104</v>
+      </c>
+      <c r="B293">
+        <v>26.83</v>
+      </c>
+      <c r="C293" s="2">
+        <v>44954</v>
+      </c>
+    </row>
+    <row r="294" spans="1:3">
+      <c r="A294" t="s">
+        <v>105</v>
+      </c>
+      <c r="B294">
+        <v>26</v>
+      </c>
+      <c r="C294" s="2">
+        <v>44744</v>
+      </c>
+    </row>
+    <row r="295" spans="1:3">
+      <c r="A295" t="s">
+        <v>105</v>
+      </c>
+      <c r="B295">
+        <v>26.73</v>
+      </c>
+      <c r="C295" s="2">
+        <v>44751</v>
+      </c>
+    </row>
+    <row r="296" spans="1:3">
+      <c r="A296" t="s">
         <v>106</v>
       </c>
-      <c r="B266">
+      <c r="B296">
+        <v>24.06</v>
+      </c>
+      <c r="C296" s="2">
+        <v>44744</v>
+      </c>
+    </row>
+    <row r="297" spans="1:3">
+      <c r="A297" t="s">
+        <v>106</v>
+      </c>
+      <c r="B297">
+        <v>24.61</v>
+      </c>
+      <c r="C297" s="2">
+        <v>44751</v>
+      </c>
+    </row>
+    <row r="298" spans="1:3">
+      <c r="A298" t="s">
+        <v>106</v>
+      </c>
+      <c r="B298">
+        <v>24.83</v>
+      </c>
+      <c r="C298" s="2">
+        <v>44814</v>
+      </c>
+    </row>
+    <row r="299" spans="1:3">
+      <c r="A299" t="s">
+        <v>106</v>
+      </c>
+      <c r="B299">
         <v>25</v>
       </c>
-      <c r="C266" s="2">
+      <c r="C299" s="2">
         <v>44940</v>
       </c>
     </row>

</xml_diff>

<commit_message>
final code for FY25 and Fy23 Labour
</commit_message>
<xml_diff>
--- a/Earliest_Pay_Rate_Changes.xlsx
+++ b/Earliest_Pay_Rate_Changes.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="113">
   <si>
     <t>Code_</t>
   </si>
@@ -28,16 +28,22 @@
     <t>ALDD</t>
   </si>
   <si>
+    <t>AMOJ</t>
+  </si>
+  <si>
     <t>ANWL</t>
   </si>
   <si>
     <t>ARMS</t>
   </si>
   <si>
+    <t>BAKA</t>
+  </si>
+  <si>
     <t>BARG</t>
   </si>
   <si>
-    <t>BARJ</t>
+    <t>BARN</t>
   </si>
   <si>
     <t>BART</t>
@@ -46,19 +52,28 @@
     <t>BEAA</t>
   </si>
   <si>
+    <t>BENJ</t>
+  </si>
+  <si>
     <t>BENL</t>
   </si>
   <si>
+    <t>BLED</t>
+  </si>
+  <si>
+    <t>BOTA</t>
+  </si>
+  <si>
+    <t>BRAL</t>
+  </si>
+  <si>
     <t>BRIT</t>
   </si>
   <si>
     <t>BROD</t>
   </si>
   <si>
-    <t>BRYJ</t>
-  </si>
-  <si>
-    <t>BURD</t>
+    <t>BYRT</t>
   </si>
   <si>
     <t>CADD</t>
@@ -67,40 +82,40 @@
     <t>CANS</t>
   </si>
   <si>
-    <t>CLAJ</t>
-  </si>
-  <si>
-    <t>COLA</t>
+    <t>CANT</t>
+  </si>
+  <si>
+    <t>CHOS</t>
+  </si>
+  <si>
+    <t>CLAB</t>
+  </si>
+  <si>
+    <t>COLD</t>
   </si>
   <si>
     <t>COLJ</t>
   </si>
   <si>
-    <t>COMI</t>
-  </si>
-  <si>
-    <t>CONM</t>
+    <t>CREN</t>
+  </si>
+  <si>
+    <t>DARM</t>
   </si>
   <si>
     <t>DAYS</t>
   </si>
   <si>
-    <t>DILR</t>
-  </si>
-  <si>
     <t>DOKI</t>
   </si>
   <si>
-    <t>DONJ</t>
-  </si>
-  <si>
     <t>DONR</t>
   </si>
   <si>
     <t>DOYF</t>
   </si>
   <si>
-    <t>DUNM</t>
+    <t>ELLJ</t>
   </si>
   <si>
     <t>ELLM</t>
@@ -112,12 +127,24 @@
     <t>ELLT</t>
   </si>
   <si>
+    <t>FALJ</t>
+  </si>
+  <si>
+    <t>FARG</t>
+  </si>
+  <si>
     <t>FERP</t>
   </si>
   <si>
     <t>FINM</t>
   </si>
   <si>
+    <t>FISJ</t>
+  </si>
+  <si>
+    <t>FOOA</t>
+  </si>
+  <si>
     <t>FRAG</t>
   </si>
   <si>
@@ -130,43 +157,31 @@
     <t>GAMR</t>
   </si>
   <si>
-    <t>GOMJ</t>
+    <t>GEEB</t>
   </si>
   <si>
     <t>GOWM</t>
   </si>
   <si>
-    <t>GRAM</t>
-  </si>
-  <si>
-    <t>GRAT</t>
-  </si>
-  <si>
-    <t>GREA</t>
-  </si>
-  <si>
-    <t>GRIG</t>
-  </si>
-  <si>
-    <t>GROA</t>
+    <t>GRAA</t>
   </si>
   <si>
     <t>HALS</t>
   </si>
   <si>
+    <t>HANM</t>
+  </si>
+  <si>
     <t>HARJ</t>
   </si>
   <si>
-    <t>HAYM</t>
-  </si>
-  <si>
-    <t>HEDR</t>
-  </si>
-  <si>
-    <t>HIGA</t>
-  </si>
-  <si>
-    <t>HUMR</t>
+    <t>HETB</t>
+  </si>
+  <si>
+    <t>HILJ</t>
+  </si>
+  <si>
+    <t>HORL</t>
   </si>
   <si>
     <t>JACG</t>
@@ -175,28 +190,37 @@
     <t>JENB</t>
   </si>
   <si>
-    <t>JOCH</t>
+    <t>JENG</t>
+  </si>
+  <si>
+    <t>JOHB</t>
+  </si>
+  <si>
+    <t>JONC</t>
   </si>
   <si>
     <t>JOND</t>
   </si>
   <si>
-    <t>JONM</t>
+    <t>JONK</t>
   </si>
   <si>
     <t>KELC</t>
   </si>
   <si>
-    <t>KOTR</t>
+    <t>KERJ</t>
+  </si>
+  <si>
+    <t>KUZP</t>
   </si>
   <si>
     <t>LABJ</t>
   </si>
   <si>
-    <t>LEEJ</t>
-  </si>
-  <si>
-    <t>LIBR</t>
+    <t>LEWA</t>
+  </si>
+  <si>
+    <t>LOHJ</t>
   </si>
   <si>
     <t>MACK</t>
@@ -205,49 +229,61 @@
     <t>MANI</t>
   </si>
   <si>
+    <t>MATT</t>
+  </si>
+  <si>
     <t>MCAA</t>
   </si>
   <si>
     <t>MCAI</t>
   </si>
   <si>
-    <t>MCCC</t>
-  </si>
-  <si>
-    <t>MCKC</t>
-  </si>
-  <si>
-    <t>MEUC</t>
-  </si>
-  <si>
-    <t>MODJ</t>
-  </si>
-  <si>
-    <t>NICR</t>
+    <t>MCKK</t>
+  </si>
+  <si>
+    <t>MERJ</t>
+  </si>
+  <si>
+    <t>NELJ</t>
+  </si>
+  <si>
+    <t>NIES</t>
+  </si>
+  <si>
+    <t>NOWD</t>
   </si>
   <si>
     <t>NUAG</t>
   </si>
   <si>
-    <t>PRIM</t>
+    <t>OBRA</t>
+  </si>
+  <si>
+    <t>POWW</t>
   </si>
   <si>
     <t>PURT</t>
   </si>
   <si>
-    <t>REAB</t>
+    <t>REAJ</t>
   </si>
   <si>
     <t>RILB</t>
   </si>
   <si>
-    <t>ROLJ</t>
+    <t>ROBA</t>
+  </si>
+  <si>
+    <t>ROXA</t>
   </si>
   <si>
     <t>RUTB</t>
   </si>
   <si>
-    <t>RUTY</t>
+    <t>RYAK</t>
+  </si>
+  <si>
+    <t>SALA</t>
   </si>
   <si>
     <t>SATS</t>
@@ -259,31 +295,31 @@
     <t>SCOC</t>
   </si>
   <si>
-    <t>SHUA</t>
-  </si>
-  <si>
-    <t>SMGE</t>
-  </si>
-  <si>
-    <t>STEJ</t>
+    <t>SHED</t>
+  </si>
+  <si>
+    <t>SIMP</t>
+  </si>
+  <si>
+    <t>STEM</t>
   </si>
   <si>
     <t>STES</t>
   </si>
   <si>
-    <t>STRG</t>
+    <t>STUZ</t>
   </si>
   <si>
     <t>SUAK</t>
   </si>
   <si>
+    <t>SUTJ</t>
+  </si>
+  <si>
     <t>SZIR</t>
   </si>
   <si>
-    <t>TAUT</t>
-  </si>
-  <si>
-    <t>TAYC</t>
+    <t>TAPR</t>
   </si>
   <si>
     <t>TOTK</t>
@@ -292,31 +328,16 @@
     <t>TOTM</t>
   </si>
   <si>
-    <t>TURP</t>
-  </si>
-  <si>
     <t>VERR</t>
   </si>
   <si>
-    <t>WALB</t>
-  </si>
-  <si>
     <t>WALJ</t>
   </si>
   <si>
-    <t>WARM</t>
-  </si>
-  <si>
-    <t>WATA</t>
-  </si>
-  <si>
-    <t>WECC</t>
-  </si>
-  <si>
-    <t>WELJ</t>
-  </si>
-  <si>
-    <t>WHYB</t>
+    <t>WALS</t>
+  </si>
+  <si>
+    <t>WATR</t>
   </si>
   <si>
     <t>WILR</t>
@@ -328,10 +349,7 @@
     <t>WOOP</t>
   </si>
   <si>
-    <t>ZAKJ</t>
-  </si>
-  <si>
-    <t>ZEIM</t>
+    <t>YOUJ</t>
   </si>
   <si>
     <t>ZYSL</t>
@@ -696,7 +714,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C299"/>
+  <dimension ref="A1:C236"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -718,10 +736,10 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>39.5</v>
+        <v>42</v>
       </c>
       <c r="C2" s="2">
-        <v>44744</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -729,10 +747,10 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C3" s="2">
-        <v>44800</v>
+        <v>45659</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -740,10 +758,10 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>18.76</v>
+        <v>32</v>
       </c>
       <c r="C4" s="2">
-        <v>44989</v>
+        <v>45450</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -751,10 +769,10 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>37.96</v>
+        <v>24.85</v>
       </c>
       <c r="C5" s="2">
-        <v>44744</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -762,10 +780,10 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>40.37</v>
+        <v>23.95</v>
       </c>
       <c r="C6" s="2">
-        <v>45059</v>
+        <v>45359</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -773,10 +791,10 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>48.08</v>
+        <v>45.42</v>
       </c>
       <c r="C7" s="2">
-        <v>44751</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -784,3211 +802,2518 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C8" s="2">
-        <v>44744</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9">
-        <v>26.73</v>
+        <v>48.08</v>
       </c>
       <c r="C9" s="2">
-        <v>44751</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B10">
-        <v>28</v>
+        <v>78.23</v>
       </c>
       <c r="C10" s="2">
-        <v>44779</v>
+        <v>45485</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>29.4</v>
+        <v>70.83</v>
       </c>
       <c r="C11" s="2">
-        <v>44835</v>
+        <v>45721</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B12">
-        <v>95.89</v>
+        <v>69.14</v>
       </c>
       <c r="C12" s="2">
-        <v>44744</v>
+        <v>45794</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B13">
-        <v>31.04</v>
+        <v>60.56</v>
       </c>
       <c r="C13" s="2">
-        <v>44744</v>
+        <v>45422</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B14">
-        <v>32.3</v>
+        <v>39.37</v>
       </c>
       <c r="C14" s="2">
-        <v>44835</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B15">
-        <v>29.27</v>
+        <v>32.3</v>
       </c>
       <c r="C15" s="2">
-        <v>44744</v>
+        <v>45450</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B16">
-        <v>29.5</v>
+        <v>32.8</v>
       </c>
       <c r="C16" s="2">
-        <v>44744</v>
+        <v>45647</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B17">
-        <v>30</v>
+        <v>37.85</v>
       </c>
       <c r="C17" s="2">
-        <v>44744</v>
+        <v>45659</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B18">
-        <v>32</v>
+        <v>42.9</v>
       </c>
       <c r="C18" s="2">
-        <v>44828</v>
+        <v>45721</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B19">
-        <v>34.32</v>
+        <v>37.85</v>
       </c>
       <c r="C19" s="2">
-        <v>44842</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B20">
-        <v>18.76</v>
+        <v>38.86</v>
       </c>
       <c r="C20" s="2">
-        <v>44891</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B21">
-        <v>34</v>
+        <v>37.35</v>
       </c>
       <c r="C21" s="2">
-        <v>44982</v>
+        <v>45485</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B22">
-        <v>32</v>
+        <v>65.61</v>
       </c>
       <c r="C22" s="2">
-        <v>44744</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B23">
-        <v>34.32</v>
+        <v>55.52</v>
       </c>
       <c r="C23" s="2">
-        <v>45038</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B24">
-        <v>27</v>
+        <v>63.09</v>
       </c>
       <c r="C24" s="2">
-        <v>45059</v>
+        <v>45721</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B25">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C25" s="2">
-        <v>44765</v>
+        <v>45471</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B26">
-        <v>486.4</v>
+        <v>43.4</v>
       </c>
       <c r="C26" s="2">
-        <v>44947</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B27">
-        <v>706.8</v>
+        <v>34.32</v>
       </c>
       <c r="C27" s="2">
-        <v>44947</v>
+        <v>45450</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B28">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C28" s="2">
-        <v>44954</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B29">
-        <v>44.65</v>
+        <v>48.86</v>
       </c>
       <c r="C29" s="2">
-        <v>44744</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B30">
-        <v>47.17</v>
+        <v>52.99</v>
       </c>
       <c r="C30" s="2">
-        <v>45059</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B31">
-        <v>47.95</v>
+        <v>30.13</v>
       </c>
       <c r="C31" s="2">
-        <v>44744</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B32">
-        <v>23.77</v>
+        <v>28.26</v>
       </c>
       <c r="C32" s="2">
-        <v>44751</v>
+        <v>45359</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="B33">
-        <v>22.66</v>
+        <v>27.23</v>
       </c>
       <c r="C33" s="2">
-        <v>45087</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B34">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C34" s="2">
-        <v>44744</v>
+        <v>45471</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B35">
-        <v>17.86</v>
+        <v>20.31</v>
       </c>
       <c r="C35" s="2">
-        <v>44744</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B36">
-        <v>18.76</v>
+        <v>17.93</v>
       </c>
       <c r="C36" s="2">
-        <v>44751</v>
+        <v>45359</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B37">
-        <v>29.27</v>
+        <v>16.34</v>
       </c>
       <c r="C37" s="2">
-        <v>44744</v>
+        <v>45450</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B38">
-        <v>32.3</v>
+        <v>65.61</v>
       </c>
       <c r="C38" s="2">
-        <v>44835</v>
+        <v>45721</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B39">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C39" s="2">
-        <v>44779</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B40">
-        <v>45.42</v>
+        <v>33</v>
       </c>
       <c r="C40" s="2">
-        <v>44744</v>
+        <v>45359</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B41">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="C41" s="2">
-        <v>44744</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B42">
-        <v>31.5</v>
+        <v>40.37</v>
       </c>
       <c r="C42" s="2">
-        <v>44835</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B43">
-        <v>15.88</v>
+        <v>32.3</v>
       </c>
       <c r="C43" s="2">
-        <v>44779</v>
+        <v>45450</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B44">
-        <v>18.76</v>
+        <v>37</v>
       </c>
       <c r="C44" s="2">
-        <v>44898</v>
+        <v>45659</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B45">
-        <v>50.47</v>
+        <v>40</v>
       </c>
       <c r="C45" s="2">
-        <v>44744</v>
+        <v>45721</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B46">
-        <v>26</v>
+        <v>50.47</v>
       </c>
       <c r="C46" s="2">
-        <v>44751</v>
+        <v>45721</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B47">
-        <v>26.73</v>
+        <v>16.3</v>
       </c>
       <c r="C47" s="2">
-        <v>44765</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B48">
-        <v>29</v>
+        <v>15.71</v>
       </c>
       <c r="C48" s="2">
-        <v>44835</v>
+        <v>45450</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B49">
-        <v>22.73</v>
+        <v>18.75</v>
       </c>
       <c r="C49" s="2">
-        <v>44744</v>
+        <v>45721</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B50">
-        <v>23.77</v>
+        <v>33.96</v>
       </c>
       <c r="C50" s="2">
-        <v>44758</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B51">
-        <v>24.59</v>
+        <v>31.5</v>
       </c>
       <c r="C51" s="2">
-        <v>44828</v>
+        <v>45359</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B52">
-        <v>26</v>
+        <v>50.47</v>
       </c>
       <c r="C52" s="2">
-        <v>44744</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B53">
-        <v>30</v>
+        <v>27.48</v>
       </c>
       <c r="C53" s="2">
-        <v>44744</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B54">
-        <v>41.8</v>
+        <v>26</v>
       </c>
       <c r="C54" s="2">
-        <v>44744</v>
+        <v>45450</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B55">
-        <v>26.73</v>
+        <v>27.23</v>
       </c>
       <c r="C55" s="2">
-        <v>44751</v>
+        <v>45482</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B56">
-        <v>28.07</v>
+        <v>45</v>
       </c>
       <c r="C56" s="2">
-        <v>44835</v>
+        <v>45659</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B57">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="C57" s="2">
-        <v>44961</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B58">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C58" s="2">
-        <v>44744</v>
+        <v>45450</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B59">
-        <v>22.73</v>
+        <v>16.3</v>
       </c>
       <c r="C59" s="2">
-        <v>44744</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B60">
-        <v>23.77</v>
+        <v>15.71</v>
       </c>
       <c r="C60" s="2">
-        <v>44751</v>
+        <v>45450</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B61">
-        <v>380.32</v>
+        <v>18.75</v>
       </c>
       <c r="C61" s="2">
-        <v>44947</v>
+        <v>45721</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B62">
-        <v>525.24</v>
+        <v>27.23</v>
       </c>
       <c r="C62" s="2">
-        <v>44947</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B63">
-        <v>24.59</v>
+        <v>26.25</v>
       </c>
       <c r="C63" s="2">
-        <v>44954</v>
+        <v>45450</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B64">
-        <v>12.38</v>
+        <v>27.48</v>
       </c>
       <c r="C64" s="2">
-        <v>44870</v>
+        <v>45659</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B65">
-        <v>30</v>
+        <v>22.41</v>
       </c>
       <c r="C65" s="2">
-        <v>44744</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="A66" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B66">
-        <v>34</v>
+        <v>20.31</v>
       </c>
       <c r="C66" s="2">
-        <v>44744</v>
+        <v>45359</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B67">
-        <v>36</v>
+        <v>16.34</v>
       </c>
       <c r="C67" s="2">
-        <v>44800</v>
+        <v>45450</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B68">
         <v>31.5</v>
       </c>
       <c r="C68" s="2">
-        <v>44835</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B69">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C69" s="2">
-        <v>44744</v>
+        <v>45471</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B70">
-        <v>60.56</v>
+        <v>17.41</v>
       </c>
       <c r="C70" s="2">
-        <v>44744</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="71" spans="1:3">
       <c r="A71" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="B71">
-        <v>37.4</v>
+        <v>40</v>
       </c>
       <c r="C71" s="2">
-        <v>44835</v>
+        <v>45660</v>
       </c>
     </row>
     <row r="72" spans="1:3">
       <c r="A72" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B72">
-        <v>65.61</v>
+        <v>42.4</v>
       </c>
       <c r="C72" s="2">
-        <v>44835</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="73" spans="1:3">
       <c r="A73" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="B73">
-        <v>65.61</v>
+        <v>20.31</v>
       </c>
       <c r="C73" s="2">
-        <v>44940</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="74" spans="1:3">
       <c r="A74" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="B74">
-        <v>15.88</v>
+        <v>18.07</v>
       </c>
       <c r="C74" s="2">
-        <v>44961</v>
+        <v>45450</v>
       </c>
     </row>
     <row r="75" spans="1:3">
       <c r="A75" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="B75">
-        <v>18.76</v>
+        <v>22.41</v>
       </c>
       <c r="C75" s="2">
-        <v>44975</v>
+        <v>45822</v>
       </c>
     </row>
     <row r="76" spans="1:3">
       <c r="A76" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="B76">
-        <v>16.34</v>
+        <v>41.38</v>
       </c>
       <c r="C76" s="2">
-        <v>45087</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="77" spans="1:3">
       <c r="A77" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="B77">
-        <v>23.38</v>
+        <v>50.47</v>
       </c>
       <c r="C77" s="2">
-        <v>44744</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="78" spans="1:3">
       <c r="A78" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="B78">
-        <v>37</v>
+        <v>75.7</v>
       </c>
       <c r="C78" s="2">
-        <v>44744</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="B79">
-        <v>24.59</v>
+        <v>39.22</v>
       </c>
       <c r="C79" s="2">
-        <v>44751</v>
+        <v>45471</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="B80">
-        <v>45.55</v>
+        <v>63.09</v>
       </c>
       <c r="C80" s="2">
-        <v>44751</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="81" spans="1:3">
       <c r="A81" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="B81">
-        <v>50.97</v>
+        <v>36.34</v>
       </c>
       <c r="C81" s="2">
-        <v>44835</v>
+        <v>45359</v>
       </c>
     </row>
     <row r="82" spans="1:3">
       <c r="A82" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="B82">
-        <v>98.36</v>
+        <v>33.81</v>
       </c>
       <c r="C82" s="2">
-        <v>44989</v>
+        <v>45471</v>
       </c>
     </row>
     <row r="83" spans="1:3">
       <c r="A83" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="B83">
-        <v>12.99</v>
+        <v>37</v>
       </c>
       <c r="C83" s="2">
-        <v>44793</v>
+        <v>45471</v>
       </c>
     </row>
     <row r="84" spans="1:3">
       <c r="A84" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="B84">
-        <v>15.88</v>
+        <v>24.85</v>
       </c>
       <c r="C84" s="2">
-        <v>44800</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="85" spans="1:3">
       <c r="A85" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="B85">
-        <v>17.5</v>
+        <v>18.76</v>
       </c>
       <c r="C85" s="2">
-        <v>44940</v>
+        <v>45359</v>
       </c>
     </row>
     <row r="86" spans="1:3">
       <c r="A86" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="B86">
-        <v>30</v>
+        <v>20.58</v>
       </c>
       <c r="C86" s="2">
-        <v>44744</v>
+        <v>45521</v>
       </c>
     </row>
     <row r="87" spans="1:3">
       <c r="A87" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="B87">
-        <v>31.5</v>
+        <v>14.25</v>
       </c>
       <c r="C87" s="2">
-        <v>44835</v>
+        <v>45640</v>
       </c>
     </row>
     <row r="88" spans="1:3">
       <c r="A88" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="B88">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C88" s="2">
-        <v>44744</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="89" spans="1:3">
       <c r="A89" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="B89">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C89" s="2">
-        <v>44744</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="90" spans="1:3">
       <c r="A90" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="B90">
-        <v>30.45</v>
+        <v>30</v>
       </c>
       <c r="C90" s="2">
-        <v>44870</v>
+        <v>45359</v>
       </c>
     </row>
     <row r="91" spans="1:3">
       <c r="A91" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="B91">
-        <v>29.27</v>
+        <v>20.58</v>
       </c>
       <c r="C91" s="2">
-        <v>44744</v>
+        <v>45660</v>
       </c>
     </row>
     <row r="92" spans="1:3">
       <c r="A92" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B92">
-        <v>32.3</v>
+        <v>39.37</v>
       </c>
       <c r="C92" s="2">
-        <v>44835</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="93" spans="1:3">
       <c r="A93" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="B93">
-        <v>25.41</v>
+        <v>32.3</v>
       </c>
       <c r="C93" s="2">
-        <v>44744</v>
+        <v>45450</v>
       </c>
     </row>
     <row r="94" spans="1:3">
       <c r="A94" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="B94">
-        <v>26.73</v>
+        <v>24.85</v>
       </c>
       <c r="C94" s="2">
-        <v>44751</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="95" spans="1:3">
       <c r="A95" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="B95">
-        <v>29</v>
+        <v>27.23</v>
       </c>
       <c r="C95" s="2">
-        <v>44982</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="96" spans="1:3">
       <c r="A96" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="B96">
-        <v>21.58</v>
+        <v>26.25</v>
       </c>
       <c r="C96" s="2">
-        <v>44744</v>
+        <v>45450</v>
       </c>
     </row>
     <row r="97" spans="1:3">
       <c r="A97" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="B97">
-        <v>22.66</v>
+        <v>27.45</v>
       </c>
       <c r="C97" s="2">
-        <v>44751</v>
+        <v>45659</v>
       </c>
     </row>
     <row r="98" spans="1:3">
       <c r="A98" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="B98">
-        <v>26.83</v>
+        <v>26.08</v>
       </c>
       <c r="C98" s="2">
-        <v>44814</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="99" spans="1:3">
       <c r="A99" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="B99">
-        <v>29</v>
+        <v>28.26</v>
       </c>
       <c r="C99" s="2">
-        <v>44982</v>
+        <v>45359</v>
       </c>
     </row>
     <row r="100" spans="1:3">
       <c r="A100" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="B100">
-        <v>37</v>
+        <v>26.98</v>
       </c>
       <c r="C100" s="2">
-        <v>44744</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="101" spans="1:3">
       <c r="A101" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="B101">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C101" s="2">
-        <v>44744</v>
+        <v>45450</v>
       </c>
     </row>
     <row r="102" spans="1:3">
       <c r="A102" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="B102">
-        <v>15.62</v>
+        <v>27.23</v>
       </c>
       <c r="C102" s="2">
-        <v>44744</v>
+        <v>45721</v>
       </c>
     </row>
     <row r="103" spans="1:3">
       <c r="A103" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="B103">
-        <v>16.34</v>
+        <v>20.58</v>
       </c>
       <c r="C103" s="2">
-        <v>44751</v>
+        <v>45962</v>
       </c>
     </row>
     <row r="104" spans="1:3">
       <c r="A104" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="B104">
-        <v>30</v>
+        <v>20.58</v>
       </c>
       <c r="C104" s="2">
-        <v>44859</v>
+        <v>45659</v>
       </c>
     </row>
     <row r="105" spans="1:3">
       <c r="A105" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="B105">
-        <v>364.64</v>
+        <v>42.9</v>
       </c>
       <c r="C105" s="2">
-        <v>44996</v>
+        <v>45450</v>
       </c>
     </row>
     <row r="106" spans="1:3">
       <c r="A106" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="B106">
-        <v>18.5</v>
+        <v>31.23</v>
       </c>
       <c r="C106" s="2">
-        <v>45003</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="107" spans="1:3">
       <c r="A107" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="B107">
-        <v>22.73</v>
+        <v>35</v>
       </c>
       <c r="C107" s="2">
-        <v>44744</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="108" spans="1:3">
       <c r="A108" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="B108">
-        <v>23.77</v>
+        <v>32</v>
       </c>
       <c r="C108" s="2">
-        <v>44751</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="109" spans="1:3">
       <c r="A109" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="B109">
-        <v>196.72</v>
+        <v>31.23</v>
       </c>
       <c r="C109" s="2">
-        <v>44947</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="110" spans="1:3">
       <c r="A110" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="B110">
-        <v>380.32</v>
+        <v>33</v>
       </c>
       <c r="C110" s="2">
-        <v>44947</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="111" spans="1:3">
       <c r="A111" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="B111">
-        <v>24.59</v>
+        <v>28.5</v>
       </c>
       <c r="C111" s="2">
-        <v>44954</v>
+        <v>45359</v>
       </c>
     </row>
     <row r="112" spans="1:3">
       <c r="A112" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="B112">
-        <v>18.76</v>
+        <v>33</v>
       </c>
       <c r="C112" s="2">
-        <v>44968</v>
+        <v>45721</v>
       </c>
     </row>
     <row r="113" spans="1:3">
       <c r="A113" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="B113">
-        <v>26.73</v>
+        <v>26</v>
       </c>
       <c r="C113" s="2">
-        <v>45031</v>
+        <v>45471</v>
       </c>
     </row>
     <row r="114" spans="1:3">
       <c r="A114" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="B114">
-        <v>23.77</v>
+        <v>80.75</v>
       </c>
       <c r="C114" s="2">
-        <v>45087</v>
+        <v>45721</v>
       </c>
     </row>
     <row r="115" spans="1:3">
       <c r="A115" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="B115">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C115" s="2">
-        <v>45003</v>
+        <v>45359</v>
       </c>
     </row>
     <row r="116" spans="1:3">
       <c r="A116" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="B116">
-        <v>15.62</v>
+        <v>32.8</v>
       </c>
       <c r="C116" s="2">
-        <v>44744</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="117" spans="1:3">
       <c r="A117" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="B117">
-        <v>16.34</v>
+        <v>30</v>
       </c>
       <c r="C117" s="2">
-        <v>44751</v>
+        <v>45450</v>
       </c>
     </row>
     <row r="118" spans="1:3">
       <c r="A118" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="B118">
-        <v>261.44</v>
+        <v>33.96</v>
       </c>
       <c r="C118" s="2">
-        <v>45017</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="119" spans="1:3">
       <c r="A119" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="B119">
-        <v>370</v>
+        <v>31</v>
       </c>
       <c r="C119" s="2">
-        <v>45017</v>
+        <v>45359</v>
       </c>
     </row>
     <row r="120" spans="1:3">
       <c r="A120" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="B120">
-        <v>18.5</v>
+        <v>28.26</v>
       </c>
       <c r="C120" s="2">
-        <v>45024</v>
+        <v>45471</v>
       </c>
     </row>
     <row r="121" spans="1:3">
       <c r="A121" t="s">
-        <v>48</v>
+        <v>65</v>
       </c>
       <c r="B121">
-        <v>549.08</v>
+        <v>30.28</v>
       </c>
       <c r="C121" s="2">
-        <v>45087</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="122" spans="1:3">
       <c r="A122" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="B122">
-        <v>15.62</v>
+        <v>30</v>
       </c>
       <c r="C122" s="2">
-        <v>44744</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="123" spans="1:3">
       <c r="A123" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="B123">
-        <v>23.77</v>
+        <v>30.13</v>
       </c>
       <c r="C123" s="2">
-        <v>44751</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="124" spans="1:3">
       <c r="A124" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="B124">
-        <v>380.32</v>
+        <v>30.23</v>
       </c>
       <c r="C124" s="2">
-        <v>44947</v>
+        <v>45450</v>
       </c>
     </row>
     <row r="125" spans="1:3">
       <c r="A125" t="s">
-        <v>49</v>
+        <v>67</v>
       </c>
       <c r="B125">
-        <v>540.98</v>
+        <v>20.58</v>
       </c>
       <c r="C125" s="2">
-        <v>44947</v>
+        <v>45359</v>
       </c>
     </row>
     <row r="126" spans="1:3">
       <c r="A126" t="s">
-        <v>49</v>
+        <v>67</v>
       </c>
       <c r="B126">
-        <v>24.59</v>
+        <v>17.93</v>
       </c>
       <c r="C126" s="2">
-        <v>44954</v>
+        <v>45546</v>
       </c>
     </row>
     <row r="127" spans="1:3">
       <c r="A127" t="s">
-        <v>50</v>
+        <v>68</v>
       </c>
       <c r="B127">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C127" s="2">
-        <v>44744</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="128" spans="1:3">
       <c r="A128" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
       <c r="B128">
-        <v>34</v>
+        <v>18.75</v>
       </c>
       <c r="C128" s="2">
-        <v>44751</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="129" spans="1:3">
       <c r="A129" t="s">
-        <v>51</v>
+        <v>69</v>
       </c>
       <c r="B129">
-        <v>30</v>
+        <v>18.07</v>
       </c>
       <c r="C129" s="2">
-        <v>44744</v>
+        <v>45450</v>
       </c>
     </row>
     <row r="130" spans="1:3">
       <c r="A130" t="s">
-        <v>51</v>
+        <v>69</v>
       </c>
       <c r="B130">
-        <v>32</v>
+        <v>60.56</v>
       </c>
       <c r="C130" s="2">
-        <v>44835</v>
+        <v>45659</v>
       </c>
     </row>
     <row r="131" spans="1:3">
       <c r="A131" t="s">
-        <v>52</v>
+        <v>70</v>
       </c>
       <c r="B131">
-        <v>26.73</v>
+        <v>20.31</v>
       </c>
       <c r="C131" s="2">
-        <v>44954</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="132" spans="1:3">
       <c r="A132" t="s">
-        <v>53</v>
+        <v>70</v>
       </c>
       <c r="B132">
-        <v>22.73</v>
+        <v>60.56</v>
       </c>
       <c r="C132" s="2">
-        <v>44744</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="133" spans="1:3">
       <c r="A133" t="s">
-        <v>53</v>
+        <v>70</v>
       </c>
       <c r="B133">
-        <v>25.41</v>
+        <v>18.07</v>
       </c>
       <c r="C133" s="2">
-        <v>44744</v>
+        <v>45450</v>
       </c>
     </row>
     <row r="134" spans="1:3">
       <c r="A134" t="s">
-        <v>53</v>
+        <v>71</v>
       </c>
       <c r="B134">
-        <v>23.77</v>
+        <v>29.33</v>
       </c>
       <c r="C134" s="2">
-        <v>44751</v>
+        <v>45422</v>
       </c>
     </row>
     <row r="135" spans="1:3">
       <c r="A135" t="s">
-        <v>53</v>
+        <v>72</v>
       </c>
       <c r="B135">
-        <v>26.73</v>
+        <v>43</v>
       </c>
       <c r="C135" s="2">
-        <v>44751</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="136" spans="1:3">
       <c r="A136" t="s">
-        <v>53</v>
+        <v>72</v>
       </c>
       <c r="B136">
-        <v>24.59</v>
+        <v>45</v>
       </c>
       <c r="C136" s="2">
-        <v>44828</v>
+        <v>45647</v>
       </c>
     </row>
     <row r="137" spans="1:3">
       <c r="A137" t="s">
-        <v>54</v>
+        <v>72</v>
       </c>
       <c r="B137">
-        <v>32</v>
+        <v>75.7</v>
       </c>
       <c r="C137" s="2">
-        <v>44744</v>
+        <v>45659</v>
       </c>
     </row>
     <row r="138" spans="1:3">
       <c r="A138" t="s">
-        <v>55</v>
+        <v>73</v>
       </c>
       <c r="B138">
-        <v>17.86</v>
+        <v>75.7</v>
       </c>
       <c r="C138" s="2">
-        <v>44744</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="139" spans="1:3">
       <c r="A139" t="s">
-        <v>55</v>
+        <v>73</v>
       </c>
       <c r="B139">
-        <v>29.27</v>
+        <v>30</v>
       </c>
       <c r="C139" s="2">
-        <v>44744</v>
+        <v>45471</v>
       </c>
     </row>
     <row r="140" spans="1:3">
       <c r="A140" t="s">
-        <v>55</v>
+        <v>74</v>
       </c>
       <c r="B140">
-        <v>16.34</v>
+        <v>22.41</v>
       </c>
       <c r="C140" s="2">
-        <v>44751</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="141" spans="1:3">
       <c r="A141" t="s">
-        <v>55</v>
+        <v>74</v>
       </c>
       <c r="B141">
-        <v>34.32</v>
+        <v>21.6</v>
       </c>
       <c r="C141" s="2">
-        <v>44835</v>
+        <v>45450</v>
       </c>
     </row>
     <row r="142" spans="1:3">
       <c r="A142" t="s">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="B142">
-        <v>28</v>
+        <v>27.23</v>
       </c>
       <c r="C142" s="2">
-        <v>44744</v>
+        <v>45675</v>
       </c>
     </row>
     <row r="143" spans="1:3">
       <c r="A143" t="s">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="B143">
-        <v>26.73</v>
+        <v>26.23</v>
       </c>
       <c r="C143" s="2">
-        <v>44765</v>
+        <v>45721</v>
       </c>
     </row>
     <row r="144" spans="1:3">
       <c r="A144" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="B144">
-        <v>24.83</v>
+        <v>40</v>
       </c>
       <c r="C144" s="2">
-        <v>44828</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="145" spans="1:3">
       <c r="A145" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="B145">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="C145" s="2">
-        <v>44947</v>
+        <v>45359</v>
       </c>
     </row>
     <row r="146" spans="1:3">
       <c r="A146" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
       <c r="B146">
-        <v>200</v>
+        <v>70.66</v>
       </c>
       <c r="C146" s="2">
-        <v>45066</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="147" spans="1:3">
       <c r="A147" t="s">
-        <v>56</v>
+        <v>77</v>
       </c>
       <c r="B147">
-        <v>894.3</v>
+        <v>30.28</v>
       </c>
       <c r="C147" s="2">
-        <v>45066</v>
+        <v>45450</v>
       </c>
     </row>
     <row r="148" spans="1:3">
       <c r="A148" t="s">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="B148">
-        <v>1132.3</v>
+        <v>70.66</v>
       </c>
       <c r="C148" s="2">
-        <v>45073</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="149" spans="1:3">
       <c r="A149" t="s">
-        <v>56</v>
+        <v>79</v>
       </c>
       <c r="B149">
-        <v>30</v>
+        <v>42.9</v>
       </c>
       <c r="C149" s="2">
-        <v>45080</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="150" spans="1:3">
       <c r="A150" t="s">
-        <v>57</v>
+        <v>79</v>
       </c>
       <c r="B150">
-        <v>36.59</v>
+        <v>44.92</v>
       </c>
       <c r="C150" s="2">
-        <v>44856</v>
+        <v>45647</v>
       </c>
     </row>
     <row r="151" spans="1:3">
       <c r="A151" t="s">
-        <v>57</v>
+        <v>80</v>
       </c>
       <c r="B151">
-        <v>1390.41</v>
+        <v>31.91</v>
       </c>
       <c r="C151" s="2">
-        <v>45080</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="152" spans="1:3">
       <c r="A152" t="s">
-        <v>58</v>
+        <v>80</v>
       </c>
       <c r="B152">
-        <v>23.77</v>
+        <v>42</v>
       </c>
       <c r="C152" s="2">
-        <v>44940</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="153" spans="1:3">
       <c r="A153" t="s">
-        <v>58</v>
+        <v>80</v>
       </c>
       <c r="B153">
-        <v>380.32</v>
+        <v>36</v>
       </c>
       <c r="C153" s="2">
-        <v>45017</v>
+        <v>45485</v>
       </c>
     </row>
     <row r="154" spans="1:3">
       <c r="A154" t="s">
-        <v>58</v>
+        <v>80</v>
       </c>
       <c r="B154">
-        <v>540.98</v>
+        <v>48</v>
       </c>
       <c r="C154" s="2">
-        <v>45017</v>
+        <v>45721</v>
       </c>
     </row>
     <row r="155" spans="1:3">
       <c r="A155" t="s">
-        <v>58</v>
+        <v>80</v>
       </c>
       <c r="B155">
-        <v>24.59</v>
+        <v>50.47</v>
       </c>
       <c r="C155" s="2">
-        <v>45024</v>
+        <v>45808</v>
       </c>
     </row>
     <row r="156" spans="1:3">
       <c r="A156" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="B156">
-        <v>30.23</v>
+        <v>51.98</v>
       </c>
       <c r="C156" s="2">
-        <v>45031</v>
+        <v>45659</v>
       </c>
     </row>
     <row r="157" spans="1:3">
       <c r="A157" t="s">
-        <v>59</v>
+        <v>82</v>
       </c>
       <c r="B157">
-        <v>28.34</v>
+        <v>43.91</v>
       </c>
       <c r="C157" s="2">
-        <v>44786</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="158" spans="1:3">
       <c r="A158" t="s">
-        <v>60</v>
+        <v>83</v>
       </c>
       <c r="B158">
-        <v>22.73</v>
+        <v>22.41</v>
       </c>
       <c r="C158" s="2">
-        <v>44744</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="159" spans="1:3">
       <c r="A159" t="s">
-        <v>60</v>
+        <v>83</v>
       </c>
       <c r="B159">
-        <v>40.49</v>
+        <v>27.23</v>
       </c>
       <c r="C159" s="2">
-        <v>44744</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="160" spans="1:3">
       <c r="A160" t="s">
-        <v>60</v>
+        <v>83</v>
       </c>
       <c r="B160">
-        <v>23.77</v>
+        <v>20.31</v>
       </c>
       <c r="C160" s="2">
-        <v>44751</v>
+        <v>45359</v>
       </c>
     </row>
     <row r="161" spans="1:3">
       <c r="A161" t="s">
-        <v>60</v>
+        <v>83</v>
       </c>
       <c r="B161">
-        <v>50.47</v>
+        <v>18.07</v>
       </c>
       <c r="C161" s="2">
-        <v>44751</v>
+        <v>45450</v>
       </c>
     </row>
     <row r="162" spans="1:3">
       <c r="A162" t="s">
-        <v>60</v>
+        <v>83</v>
       </c>
       <c r="B162">
-        <v>12.99</v>
+        <v>26.25</v>
       </c>
       <c r="C162" s="2">
-        <v>44765</v>
+        <v>45450</v>
       </c>
     </row>
     <row r="163" spans="1:3">
       <c r="A163" t="s">
-        <v>61</v>
+        <v>84</v>
       </c>
       <c r="B163">
-        <v>12.99</v>
+        <v>26.98</v>
       </c>
       <c r="C163" s="2">
-        <v>44940</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="164" spans="1:3">
       <c r="A164" t="s">
-        <v>61</v>
+        <v>84</v>
       </c>
       <c r="B164">
-        <v>16.34</v>
+        <v>26</v>
       </c>
       <c r="C164" s="2">
-        <v>45038</v>
+        <v>45450</v>
       </c>
     </row>
     <row r="165" spans="1:3">
       <c r="A165" t="s">
-        <v>62</v>
+        <v>84</v>
       </c>
       <c r="B165">
-        <v>50.47</v>
+        <v>27.23</v>
       </c>
       <c r="C165" s="2">
-        <v>44933</v>
+        <v>45660</v>
       </c>
     </row>
     <row r="166" spans="1:3">
       <c r="A166" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="B166">
-        <v>18.76</v>
+        <v>32.8</v>
       </c>
       <c r="C166" s="2">
-        <v>44961</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="167" spans="1:3">
       <c r="A167" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="B167">
-        <v>16.34</v>
+        <v>47.95</v>
       </c>
       <c r="C167" s="2">
-        <v>44968</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="168" spans="1:3">
       <c r="A168" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="B168">
-        <v>55.52</v>
+        <v>26.98</v>
       </c>
       <c r="C168" s="2">
-        <v>45101</v>
+        <v>45659</v>
       </c>
     </row>
     <row r="169" spans="1:3">
       <c r="A169" t="s">
-        <v>63</v>
+        <v>87</v>
       </c>
       <c r="B169">
-        <v>41</v>
+        <v>26.98</v>
       </c>
       <c r="C169" s="2">
-        <v>44772</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="170" spans="1:3">
       <c r="A170" t="s">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="B170">
-        <v>30</v>
+        <v>20.31</v>
       </c>
       <c r="C170" s="2">
-        <v>44744</v>
+        <v>45359</v>
       </c>
     </row>
     <row r="171" spans="1:3">
       <c r="A171" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="B171">
-        <v>15.11</v>
+        <v>18.07</v>
       </c>
       <c r="C171" s="2">
-        <v>44744</v>
+        <v>45450</v>
       </c>
     </row>
     <row r="172" spans="1:3">
       <c r="A172" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="B172">
-        <v>32</v>
+        <v>31.5</v>
       </c>
       <c r="C172" s="2">
-        <v>44744</v>
+        <v>45450</v>
       </c>
     </row>
     <row r="173" spans="1:3">
       <c r="A173" t="s">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="B173">
-        <v>16.34</v>
+        <v>60.56</v>
       </c>
       <c r="C173" s="2">
-        <v>44751</v>
+        <v>45359</v>
       </c>
     </row>
     <row r="174" spans="1:3">
       <c r="A174" t="s">
-        <v>65</v>
+        <v>89</v>
       </c>
       <c r="B174">
-        <v>477.95</v>
+        <v>78.23</v>
       </c>
       <c r="C174" s="2">
-        <v>45010</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="175" spans="1:3">
       <c r="A175" t="s">
-        <v>65</v>
+        <v>90</v>
       </c>
       <c r="B175">
-        <v>15.88</v>
+        <v>26.98</v>
       </c>
       <c r="C175" s="2">
-        <v>45017</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="176" spans="1:3">
       <c r="A176" t="s">
-        <v>65</v>
+        <v>90</v>
       </c>
       <c r="B176">
-        <v>18.76</v>
+        <v>26</v>
       </c>
       <c r="C176" s="2">
-        <v>45024</v>
+        <v>45450</v>
       </c>
     </row>
     <row r="177" spans="1:3">
       <c r="A177" t="s">
-        <v>65</v>
+        <v>90</v>
       </c>
       <c r="B177">
-        <v>-972.8</v>
+        <v>27.23</v>
       </c>
       <c r="C177" s="2">
-        <v>45045</v>
+        <v>45721</v>
       </c>
     </row>
     <row r="178" spans="1:3">
       <c r="A178" t="s">
-        <v>66</v>
+        <v>91</v>
       </c>
       <c r="B178">
-        <v>15.62</v>
+        <v>32</v>
       </c>
       <c r="C178" s="2">
-        <v>44744</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="179" spans="1:3">
       <c r="A179" t="s">
-        <v>66</v>
+        <v>91</v>
       </c>
       <c r="B179">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C179" s="2">
-        <v>44744</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="180" spans="1:3">
       <c r="A180" t="s">
-        <v>66</v>
+        <v>92</v>
       </c>
       <c r="B180">
-        <v>16.34</v>
+        <v>42.9</v>
       </c>
       <c r="C180" s="2">
-        <v>44751</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="181" spans="1:3">
       <c r="A181" t="s">
-        <v>66</v>
+        <v>92</v>
       </c>
       <c r="B181">
-        <v>31.5</v>
+        <v>45.93</v>
       </c>
       <c r="C181" s="2">
-        <v>44835</v>
+        <v>45485</v>
       </c>
     </row>
     <row r="182" spans="1:3">
       <c r="A182" t="s">
-        <v>66</v>
+        <v>92</v>
       </c>
       <c r="B182">
-        <v>130.72</v>
+        <v>36</v>
       </c>
       <c r="C182" s="2">
-        <v>45017</v>
+        <v>45659</v>
       </c>
     </row>
     <row r="183" spans="1:3">
       <c r="A183" t="s">
-        <v>66</v>
+        <v>92</v>
       </c>
       <c r="B183">
-        <v>407</v>
+        <v>38.5</v>
       </c>
       <c r="C183" s="2">
-        <v>45017</v>
+        <v>45659</v>
       </c>
     </row>
     <row r="184" spans="1:3">
       <c r="A184" t="s">
-        <v>66</v>
+        <v>92</v>
       </c>
       <c r="B184">
-        <v>18.5</v>
+        <v>38</v>
       </c>
       <c r="C184" s="2">
-        <v>45024</v>
+        <v>45721</v>
       </c>
     </row>
     <row r="185" spans="1:3">
       <c r="A185" t="s">
-        <v>67</v>
+        <v>93</v>
       </c>
       <c r="B185">
-        <v>26.73</v>
+        <v>36</v>
       </c>
       <c r="C185" s="2">
-        <v>44758</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="186" spans="1:3">
       <c r="A186" t="s">
-        <v>67</v>
+        <v>93</v>
       </c>
       <c r="B186">
-        <v>60.56</v>
+        <v>38.5</v>
       </c>
       <c r="C186" s="2">
-        <v>44940</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="187" spans="1:3">
       <c r="A187" t="s">
-        <v>67</v>
+        <v>93</v>
       </c>
       <c r="B187">
-        <v>30</v>
+        <v>19.84</v>
       </c>
       <c r="C187" s="2">
-        <v>44968</v>
+        <v>45359</v>
       </c>
     </row>
     <row r="188" spans="1:3">
       <c r="A188" t="s">
-        <v>68</v>
+        <v>93</v>
       </c>
       <c r="B188">
-        <v>22.73</v>
+        <v>20.58</v>
       </c>
       <c r="C188" s="2">
-        <v>44744</v>
+        <v>45482</v>
       </c>
     </row>
     <row r="189" spans="1:3">
       <c r="A189" t="s">
-        <v>68</v>
+        <v>94</v>
       </c>
       <c r="B189">
-        <v>34</v>
+        <v>58.04</v>
       </c>
       <c r="C189" s="2">
-        <v>44744</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="190" spans="1:3">
       <c r="A190" t="s">
-        <v>68</v>
+        <v>94</v>
       </c>
       <c r="B190">
-        <v>54.66</v>
+        <v>35</v>
       </c>
       <c r="C190" s="2">
-        <v>44744</v>
+        <v>45822</v>
       </c>
     </row>
     <row r="191" spans="1:3">
       <c r="A191" t="s">
-        <v>68</v>
+        <v>95</v>
       </c>
       <c r="B191">
-        <v>70.66</v>
+        <v>17.93</v>
       </c>
       <c r="C191" s="2">
-        <v>44744</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="192" spans="1:3">
       <c r="A192" t="s">
-        <v>68</v>
+        <v>95</v>
       </c>
       <c r="B192">
-        <v>23.77</v>
+        <v>15.71</v>
       </c>
       <c r="C192" s="2">
-        <v>44751</v>
+        <v>45450</v>
       </c>
     </row>
     <row r="193" spans="1:3">
       <c r="A193" t="s">
-        <v>68</v>
+        <v>95</v>
       </c>
       <c r="B193">
-        <v>60.56</v>
+        <v>20.31</v>
       </c>
       <c r="C193" s="2">
-        <v>44835</v>
+        <v>45721</v>
       </c>
     </row>
     <row r="194" spans="1:3">
       <c r="A194" t="s">
-        <v>69</v>
+        <v>96</v>
       </c>
       <c r="B194">
-        <v>70.66</v>
+        <v>60.56</v>
       </c>
       <c r="C194" s="2">
-        <v>44933</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="195" spans="1:3">
       <c r="A195" t="s">
-        <v>69</v>
+        <v>97</v>
       </c>
       <c r="B195">
-        <v>15.88</v>
+        <v>14.25</v>
       </c>
       <c r="C195" s="2">
-        <v>44982</v>
+        <v>45659</v>
       </c>
     </row>
     <row r="196" spans="1:3">
       <c r="A196" t="s">
-        <v>69</v>
+        <v>98</v>
       </c>
       <c r="B196">
-        <v>16.34</v>
+        <v>34</v>
       </c>
       <c r="C196" s="2">
-        <v>45087</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="197" spans="1:3">
       <c r="A197" t="s">
-        <v>70</v>
+        <v>98</v>
       </c>
       <c r="B197">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C197" s="2">
-        <v>44744</v>
+        <v>45359</v>
       </c>
     </row>
     <row r="198" spans="1:3">
       <c r="A198" t="s">
-        <v>70</v>
+        <v>99</v>
       </c>
       <c r="B198">
-        <v>42.9</v>
+        <v>22.41</v>
       </c>
       <c r="C198" s="2">
-        <v>44744</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="199" spans="1:3">
       <c r="A199" t="s">
-        <v>70</v>
+        <v>99</v>
       </c>
       <c r="B199">
-        <v>37</v>
+        <v>20.31</v>
       </c>
       <c r="C199" s="2">
-        <v>44828</v>
+        <v>45359</v>
       </c>
     </row>
     <row r="200" spans="1:3">
       <c r="A200" t="s">
-        <v>71</v>
+        <v>99</v>
       </c>
       <c r="B200">
-        <v>42.9</v>
+        <v>18.07</v>
       </c>
       <c r="C200" s="2">
-        <v>44744</v>
+        <v>45450</v>
       </c>
     </row>
     <row r="201" spans="1:3">
       <c r="A201" t="s">
-        <v>71</v>
+        <v>99</v>
       </c>
       <c r="B201">
-        <v>1630.14</v>
+        <v>27.23</v>
       </c>
       <c r="C201" s="2">
-        <v>44996</v>
+        <v>45675</v>
       </c>
     </row>
     <row r="202" spans="1:3">
       <c r="A202" t="s">
-        <v>72</v>
+        <v>100</v>
       </c>
       <c r="B202">
-        <v>35.33</v>
+        <v>27.23</v>
       </c>
       <c r="C202" s="2">
-        <v>44744</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="203" spans="1:3">
       <c r="A203" t="s">
-        <v>72</v>
+        <v>100</v>
       </c>
       <c r="B203">
-        <v>37.85</v>
+        <v>26.25</v>
       </c>
       <c r="C203" s="2">
-        <v>44947</v>
+        <v>45450</v>
       </c>
     </row>
     <row r="204" spans="1:3">
       <c r="A204" t="s">
-        <v>72</v>
+        <v>100</v>
       </c>
       <c r="B204">
-        <v>39.11</v>
+        <v>30.13</v>
       </c>
       <c r="C204" s="2">
-        <v>45059</v>
+        <v>45659</v>
       </c>
     </row>
     <row r="205" spans="1:3">
       <c r="A205" t="s">
-        <v>73</v>
+        <v>100</v>
       </c>
       <c r="B205">
-        <v>17.86</v>
+        <v>37</v>
       </c>
       <c r="C205" s="2">
-        <v>44744</v>
+        <v>45659</v>
       </c>
     </row>
     <row r="206" spans="1:3">
       <c r="A206" t="s">
-        <v>73</v>
+        <v>100</v>
       </c>
       <c r="B206">
-        <v>22.73</v>
+        <v>27.48</v>
       </c>
       <c r="C206" s="2">
-        <v>44744</v>
+        <v>45721</v>
       </c>
     </row>
     <row r="207" spans="1:3">
       <c r="A207" t="s">
-        <v>73</v>
+        <v>101</v>
       </c>
       <c r="B207">
-        <v>18.76</v>
+        <v>30.13</v>
       </c>
       <c r="C207" s="2">
-        <v>44751</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="208" spans="1:3">
       <c r="A208" t="s">
-        <v>73</v>
+        <v>101</v>
       </c>
       <c r="B208">
-        <v>23.77</v>
+        <v>35</v>
       </c>
       <c r="C208" s="2">
-        <v>44751</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="209" spans="1:3">
       <c r="A209" t="s">
-        <v>73</v>
+        <v>101</v>
       </c>
       <c r="B209">
-        <v>16.34</v>
+        <v>28.26</v>
       </c>
       <c r="C209" s="2">
-        <v>44835</v>
+        <v>45450</v>
       </c>
     </row>
     <row r="210" spans="1:3">
       <c r="A210" t="s">
-        <v>73</v>
+        <v>101</v>
       </c>
       <c r="B210">
-        <v>14.23</v>
+        <v>37</v>
       </c>
       <c r="C210" s="2">
-        <v>44898</v>
+        <v>45485</v>
       </c>
     </row>
     <row r="211" spans="1:3">
       <c r="A211" t="s">
-        <v>73</v>
+        <v>102</v>
       </c>
       <c r="B211">
-        <v>17.08</v>
+        <v>30.13</v>
       </c>
       <c r="C211" s="2">
-        <v>44905</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="212" spans="1:3">
       <c r="A212" t="s">
-        <v>73</v>
+        <v>102</v>
       </c>
       <c r="B212">
-        <v>380.32</v>
+        <v>28.5</v>
       </c>
       <c r="C212" s="2">
-        <v>45017</v>
+        <v>45359</v>
       </c>
     </row>
     <row r="213" spans="1:3">
       <c r="A213" t="s">
-        <v>73</v>
+        <v>103</v>
       </c>
       <c r="B213">
-        <v>540.98</v>
+        <v>16.3</v>
       </c>
       <c r="C213" s="2">
-        <v>45017</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="214" spans="1:3">
       <c r="A214" t="s">
-        <v>73</v>
+        <v>103</v>
       </c>
       <c r="B214">
-        <v>24.59</v>
+        <v>34</v>
       </c>
       <c r="C214" s="2">
-        <v>45024</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="215" spans="1:3">
       <c r="A215" t="s">
-        <v>74</v>
+        <v>103</v>
       </c>
       <c r="B215">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="C215" s="2">
-        <v>44744</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="216" spans="1:3">
       <c r="A216" t="s">
-        <v>74</v>
+        <v>103</v>
       </c>
       <c r="B216">
-        <v>26.73</v>
+        <v>14.25</v>
       </c>
       <c r="C216" s="2">
-        <v>44765</v>
+        <v>45359</v>
       </c>
     </row>
     <row r="217" spans="1:3">
       <c r="A217" t="s">
-        <v>74</v>
+        <v>103</v>
       </c>
       <c r="B217">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C217" s="2">
-        <v>44835</v>
+        <v>45359</v>
       </c>
     </row>
     <row r="218" spans="1:3">
       <c r="A218" t="s">
-        <v>74</v>
+        <v>104</v>
       </c>
       <c r="B218">
-        <v>23.77</v>
+        <v>22.41</v>
       </c>
       <c r="C218" s="2">
-        <v>44968</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="219" spans="1:3">
       <c r="A219" t="s">
-        <v>75</v>
+        <v>104</v>
       </c>
       <c r="B219">
-        <v>35</v>
+        <v>21.6</v>
       </c>
       <c r="C219" s="2">
-        <v>44933</v>
+        <v>45450</v>
       </c>
     </row>
     <row r="220" spans="1:3">
       <c r="A220" t="s">
-        <v>75</v>
+        <v>104</v>
       </c>
       <c r="B220">
-        <v>26.73</v>
+        <v>70.66</v>
       </c>
       <c r="C220" s="2">
-        <v>44968</v>
+        <v>45485</v>
       </c>
     </row>
     <row r="221" spans="1:3">
       <c r="A221" t="s">
-        <v>75</v>
+        <v>104</v>
       </c>
       <c r="B221">
-        <v>23.77</v>
+        <v>26.23</v>
       </c>
       <c r="C221" s="2">
-        <v>45087</v>
+        <v>45721</v>
       </c>
     </row>
     <row r="222" spans="1:3">
       <c r="A222" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="B222">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C222" s="2">
-        <v>44744</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="223" spans="1:3">
       <c r="A223" t="s">
-        <v>76</v>
+        <v>106</v>
       </c>
       <c r="B223">
-        <v>31.5</v>
+        <v>17.93</v>
       </c>
       <c r="C223" s="2">
-        <v>44835</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="224" spans="1:3">
       <c r="A224" t="s">
-        <v>77</v>
+        <v>106</v>
       </c>
       <c r="B224">
-        <v>17.86</v>
+        <v>15.71</v>
       </c>
       <c r="C224" s="2">
-        <v>44744</v>
+        <v>45450</v>
       </c>
     </row>
     <row r="225" spans="1:3">
       <c r="A225" t="s">
-        <v>77</v>
+        <v>106</v>
       </c>
       <c r="B225">
-        <v>28.5</v>
+        <v>32</v>
       </c>
       <c r="C225" s="2">
-        <v>44744</v>
+        <v>45485</v>
       </c>
     </row>
     <row r="226" spans="1:3">
       <c r="A226" t="s">
-        <v>77</v>
+        <v>106</v>
       </c>
       <c r="B226">
-        <v>18.76</v>
+        <v>20.31</v>
       </c>
       <c r="C226" s="2">
-        <v>44751</v>
+        <v>45721</v>
       </c>
     </row>
     <row r="227" spans="1:3">
       <c r="A227" t="s">
-        <v>77</v>
+        <v>107</v>
       </c>
       <c r="B227">
-        <v>22.66</v>
+        <v>40.37</v>
       </c>
       <c r="C227" s="2">
-        <v>44779</v>
+        <v>45359</v>
       </c>
     </row>
     <row r="228" spans="1:3">
       <c r="A228" t="s">
-        <v>77</v>
+        <v>108</v>
       </c>
       <c r="B228">
-        <v>16.34</v>
+        <v>52.99</v>
       </c>
       <c r="C228" s="2">
-        <v>44982</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="229" spans="1:3">
       <c r="A229" t="s">
-        <v>78</v>
+        <v>109</v>
       </c>
       <c r="B229">
-        <v>26.73</v>
+        <v>37.35</v>
       </c>
       <c r="C229" s="2">
-        <v>44940</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="230" spans="1:3">
       <c r="A230" t="s">
-        <v>78</v>
+        <v>109</v>
       </c>
       <c r="B230">
-        <v>23.77</v>
+        <v>31.29</v>
       </c>
       <c r="C230" s="2">
-        <v>45038</v>
+        <v>45450</v>
       </c>
     </row>
     <row r="231" spans="1:3">
       <c r="A231" t="s">
-        <v>79</v>
+        <v>110</v>
       </c>
       <c r="B231">
-        <v>28</v>
+        <v>45.42</v>
       </c>
       <c r="C231" s="2">
-        <v>44744</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="232" spans="1:3">
       <c r="A232" t="s">
-        <v>79</v>
+        <v>110</v>
       </c>
       <c r="B232">
-        <v>30</v>
+        <v>28.38</v>
       </c>
       <c r="C232" s="2">
-        <v>44856</v>
+        <v>45359</v>
       </c>
     </row>
     <row r="233" spans="1:3">
       <c r="A233" t="s">
-        <v>79</v>
+        <v>111</v>
       </c>
       <c r="B233">
-        <v>35</v>
+        <v>17.93</v>
       </c>
       <c r="C233" s="2">
-        <v>45087</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="234" spans="1:3">
       <c r="A234" t="s">
-        <v>80</v>
+        <v>111</v>
       </c>
       <c r="B234">
-        <v>37.85</v>
+        <v>15.71</v>
       </c>
       <c r="C234" s="2">
-        <v>44744</v>
+        <v>45450</v>
       </c>
     </row>
     <row r="235" spans="1:3">
       <c r="A235" t="s">
-        <v>80</v>
+        <v>111</v>
       </c>
       <c r="B235">
-        <v>42.9</v>
+        <v>20.31</v>
       </c>
       <c r="C235" s="2">
-        <v>45101</v>
+        <v>45660</v>
       </c>
     </row>
     <row r="236" spans="1:3">
       <c r="A236" t="s">
-        <v>81</v>
+        <v>112</v>
       </c>
       <c r="B236">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C236" s="2">
-        <v>44744</v>
-      </c>
-    </row>
-    <row r="237" spans="1:3">
-      <c r="A237" t="s">
-        <v>81</v>
-      </c>
-      <c r="B237">
-        <v>26.73</v>
-      </c>
-      <c r="C237" s="2">
-        <v>44800</v>
-      </c>
-    </row>
-    <row r="238" spans="1:3">
-      <c r="A238" t="s">
-        <v>81</v>
-      </c>
-      <c r="B238">
-        <v>24.59</v>
-      </c>
-      <c r="C238" s="2">
-        <v>44828</v>
-      </c>
-    </row>
-    <row r="239" spans="1:3">
-      <c r="A239" t="s">
-        <v>82</v>
-      </c>
-      <c r="B239">
-        <v>31</v>
-      </c>
-      <c r="C239" s="2">
-        <v>44940</v>
-      </c>
-    </row>
-    <row r="240" spans="1:3">
-      <c r="A240" t="s">
-        <v>82</v>
-      </c>
-      <c r="B240">
-        <v>22.66</v>
-      </c>
-      <c r="C240" s="2">
-        <v>45073</v>
-      </c>
-    </row>
-    <row r="241" spans="1:3">
-      <c r="A241" t="s">
-        <v>83</v>
-      </c>
-      <c r="B241">
-        <v>17.86</v>
-      </c>
-      <c r="C241" s="2">
-        <v>44744</v>
-      </c>
-    </row>
-    <row r="242" spans="1:3">
-      <c r="A242" t="s">
-        <v>83</v>
-      </c>
-      <c r="B242">
-        <v>18.76</v>
-      </c>
-      <c r="C242" s="2">
-        <v>44751</v>
-      </c>
-    </row>
-    <row r="243" spans="1:3">
-      <c r="A243" t="s">
-        <v>83</v>
-      </c>
-      <c r="B243">
-        <v>22.66</v>
-      </c>
-      <c r="C243" s="2">
-        <v>44779</v>
-      </c>
-    </row>
-    <row r="244" spans="1:3">
-      <c r="A244" t="s">
-        <v>83</v>
-      </c>
-      <c r="B244">
-        <v>26</v>
-      </c>
-      <c r="C244" s="2">
-        <v>44835</v>
-      </c>
-    </row>
-    <row r="245" spans="1:3">
-      <c r="A245" t="s">
-        <v>84</v>
-      </c>
-      <c r="B245">
-        <v>50.61</v>
-      </c>
-      <c r="C245" s="2">
-        <v>44744</v>
-      </c>
-    </row>
-    <row r="246" spans="1:3">
-      <c r="A246" t="s">
-        <v>84</v>
-      </c>
-      <c r="B246">
-        <v>60.56</v>
-      </c>
-      <c r="C246" s="2">
-        <v>44835</v>
-      </c>
-    </row>
-    <row r="247" spans="1:3">
-      <c r="A247" t="s">
-        <v>85</v>
-      </c>
-      <c r="B247">
-        <v>55.52</v>
-      </c>
-      <c r="C247" s="2">
-        <v>44744</v>
-      </c>
-    </row>
-    <row r="248" spans="1:3">
-      <c r="A248" t="s">
-        <v>86</v>
-      </c>
-      <c r="B248">
-        <v>17.86</v>
-      </c>
-      <c r="C248" s="2">
-        <v>44744</v>
-      </c>
-    </row>
-    <row r="249" spans="1:3">
-      <c r="A249" t="s">
-        <v>86</v>
-      </c>
-      <c r="B249">
-        <v>32</v>
-      </c>
-      <c r="C249" s="2">
-        <v>44744</v>
-      </c>
-    </row>
-    <row r="250" spans="1:3">
-      <c r="A250" t="s">
-        <v>86</v>
-      </c>
-      <c r="B250">
-        <v>18.76</v>
-      </c>
-      <c r="C250" s="2">
-        <v>44751</v>
-      </c>
-    </row>
-    <row r="251" spans="1:3">
-      <c r="A251" t="s">
-        <v>86</v>
-      </c>
-      <c r="B251">
-        <v>16.34</v>
-      </c>
-      <c r="C251" s="2">
-        <v>44835</v>
-      </c>
-    </row>
-    <row r="252" spans="1:3">
-      <c r="A252" t="s">
-        <v>87</v>
-      </c>
-      <c r="B252">
-        <v>15.62</v>
-      </c>
-      <c r="C252" s="2">
-        <v>44744</v>
-      </c>
-    </row>
-    <row r="253" spans="1:3">
-      <c r="A253" t="s">
-        <v>87</v>
-      </c>
-      <c r="B253">
-        <v>16.34</v>
-      </c>
-      <c r="C253" s="2">
-        <v>44751</v>
-      </c>
-    </row>
-    <row r="254" spans="1:3">
-      <c r="A254" t="s">
-        <v>87</v>
-      </c>
-      <c r="B254">
-        <v>23.77</v>
-      </c>
-      <c r="C254" s="2">
-        <v>44821</v>
-      </c>
-    </row>
-    <row r="255" spans="1:3">
-      <c r="A255" t="s">
-        <v>87</v>
-      </c>
-      <c r="B255">
-        <v>350.41</v>
-      </c>
-      <c r="C255" s="2">
-        <v>44996</v>
-      </c>
-    </row>
-    <row r="256" spans="1:3">
-      <c r="A256" t="s">
-        <v>87</v>
-      </c>
-      <c r="B256">
-        <v>361.3</v>
-      </c>
-      <c r="C256" s="2">
-        <v>44996</v>
-      </c>
-    </row>
-    <row r="257" spans="1:3">
-      <c r="A257" t="s">
-        <v>87</v>
-      </c>
-      <c r="B257">
-        <v>24.59</v>
-      </c>
-      <c r="C257" s="2">
-        <v>45003</v>
-      </c>
-    </row>
-    <row r="258" spans="1:3">
-      <c r="A258" t="s">
-        <v>88</v>
-      </c>
-      <c r="B258">
-        <v>25.41</v>
-      </c>
-      <c r="C258" s="2">
-        <v>44744</v>
-      </c>
-    </row>
-    <row r="259" spans="1:3">
-      <c r="A259" t="s">
-        <v>88</v>
-      </c>
-      <c r="B259">
-        <v>26.73</v>
-      </c>
-      <c r="C259" s="2">
-        <v>44751</v>
-      </c>
-    </row>
-    <row r="260" spans="1:3">
-      <c r="A260" t="s">
-        <v>88</v>
-      </c>
-      <c r="B260">
-        <v>35</v>
-      </c>
-      <c r="C260" s="2">
-        <v>45087</v>
-      </c>
-    </row>
-    <row r="261" spans="1:3">
-      <c r="A261" t="s">
-        <v>89</v>
-      </c>
-      <c r="B261">
-        <v>30.95</v>
-      </c>
-      <c r="C261" s="2">
-        <v>44751</v>
-      </c>
-    </row>
-    <row r="262" spans="1:3">
-      <c r="A262" t="s">
-        <v>90</v>
-      </c>
-      <c r="B262">
-        <v>25.41</v>
-      </c>
-      <c r="C262" s="2">
-        <v>44744</v>
-      </c>
-    </row>
-    <row r="263" spans="1:3">
-      <c r="A263" t="s">
-        <v>90</v>
-      </c>
-      <c r="B263">
-        <v>26.73</v>
-      </c>
-      <c r="C263" s="2">
-        <v>44751</v>
-      </c>
-    </row>
-    <row r="264" spans="1:3">
-      <c r="A264" t="s">
-        <v>91</v>
-      </c>
-      <c r="B264">
-        <v>38</v>
-      </c>
-      <c r="C264" s="2">
-        <v>44744</v>
-      </c>
-    </row>
-    <row r="265" spans="1:3">
-      <c r="A265" t="s">
-        <v>92</v>
-      </c>
-      <c r="B265">
-        <v>28.08</v>
-      </c>
-      <c r="C265" s="2">
-        <v>44744</v>
-      </c>
-    </row>
-    <row r="266" spans="1:3">
-      <c r="A266" t="s">
-        <v>92</v>
-      </c>
-      <c r="B266">
-        <v>29.39</v>
-      </c>
-      <c r="C266" s="2">
-        <v>44758</v>
-      </c>
-    </row>
-    <row r="267" spans="1:3">
-      <c r="A267" t="s">
-        <v>93</v>
-      </c>
-      <c r="B267">
-        <v>15.62</v>
-      </c>
-      <c r="C267" s="2">
-        <v>44744</v>
-      </c>
-    </row>
-    <row r="268" spans="1:3">
-      <c r="A268" t="s">
-        <v>93</v>
-      </c>
-      <c r="B268">
-        <v>16.34</v>
-      </c>
-      <c r="C268" s="2">
-        <v>44751</v>
-      </c>
-    </row>
-    <row r="269" spans="1:3">
-      <c r="A269" t="s">
-        <v>93</v>
-      </c>
-      <c r="B269">
-        <v>130.72</v>
-      </c>
-      <c r="C269" s="2">
-        <v>45017</v>
-      </c>
-    </row>
-    <row r="270" spans="1:3">
-      <c r="A270" t="s">
-        <v>93</v>
-      </c>
-      <c r="B270">
-        <v>407</v>
-      </c>
-      <c r="C270" s="2">
-        <v>45017</v>
-      </c>
-    </row>
-    <row r="271" spans="1:3">
-      <c r="A271" t="s">
-        <v>93</v>
-      </c>
-      <c r="B271">
-        <v>18.5</v>
-      </c>
-      <c r="C271" s="2">
-        <v>45024</v>
-      </c>
-    </row>
-    <row r="272" spans="1:3">
-      <c r="A272" t="s">
-        <v>94</v>
-      </c>
-      <c r="B272">
-        <v>32</v>
-      </c>
-      <c r="C272" s="2">
-        <v>44744</v>
-      </c>
-    </row>
-    <row r="273" spans="1:3">
-      <c r="A273" t="s">
-        <v>94</v>
-      </c>
-      <c r="B273">
-        <v>34</v>
-      </c>
-      <c r="C273" s="2">
-        <v>44779</v>
-      </c>
-    </row>
-    <row r="274" spans="1:3">
-      <c r="A274" t="s">
-        <v>95</v>
-      </c>
-      <c r="B274">
-        <v>35</v>
-      </c>
-      <c r="C274" s="2">
-        <v>44772</v>
-      </c>
-    </row>
-    <row r="275" spans="1:3">
-      <c r="A275" t="s">
-        <v>96</v>
-      </c>
-      <c r="B275">
-        <v>24.32</v>
-      </c>
-      <c r="C275" s="2">
-        <v>44744</v>
-      </c>
-    </row>
-    <row r="276" spans="1:3">
-      <c r="A276" t="s">
-        <v>96</v>
-      </c>
-      <c r="B276">
-        <v>25.05</v>
-      </c>
-      <c r="C276" s="2">
-        <v>44751</v>
-      </c>
-    </row>
-    <row r="277" spans="1:3">
-      <c r="A277" t="s">
-        <v>96</v>
-      </c>
-      <c r="B277">
-        <v>31</v>
-      </c>
-      <c r="C277" s="2">
-        <v>44863</v>
-      </c>
-    </row>
-    <row r="278" spans="1:3">
-      <c r="A278" t="s">
-        <v>96</v>
-      </c>
-      <c r="B278">
-        <v>1085.62</v>
-      </c>
-      <c r="C278" s="2">
-        <v>44961</v>
-      </c>
-    </row>
-    <row r="279" spans="1:3">
-      <c r="A279" t="s">
-        <v>97</v>
-      </c>
-      <c r="B279">
-        <v>25.41</v>
-      </c>
-      <c r="C279" s="2">
-        <v>44744</v>
-      </c>
-    </row>
-    <row r="280" spans="1:3">
-      <c r="A280" t="s">
-        <v>97</v>
-      </c>
-      <c r="B280">
-        <v>23.77</v>
-      </c>
-      <c r="C280" s="2">
-        <v>44751</v>
-      </c>
-    </row>
-    <row r="281" spans="1:3">
-      <c r="A281" t="s">
-        <v>98</v>
-      </c>
-      <c r="B281">
-        <v>26.73</v>
-      </c>
-      <c r="C281" s="2">
-        <v>44982</v>
-      </c>
-    </row>
-    <row r="282" spans="1:3">
-      <c r="A282" t="s">
-        <v>98</v>
-      </c>
-      <c r="B282">
-        <v>28.5</v>
-      </c>
-      <c r="C282" s="2">
-        <v>45059</v>
-      </c>
-    </row>
-    <row r="283" spans="1:3">
-      <c r="A283" t="s">
-        <v>99</v>
-      </c>
-      <c r="B283">
-        <v>25.41</v>
-      </c>
-      <c r="C283" s="2">
-        <v>44744</v>
-      </c>
-    </row>
-    <row r="284" spans="1:3">
-      <c r="A284" t="s">
-        <v>99</v>
-      </c>
-      <c r="B284">
-        <v>26.73</v>
-      </c>
-      <c r="C284" s="2">
-        <v>44751</v>
-      </c>
-    </row>
-    <row r="285" spans="1:3">
-      <c r="A285" t="s">
-        <v>100</v>
-      </c>
-      <c r="B285">
-        <v>28</v>
-      </c>
-      <c r="C285" s="2">
-        <v>44744</v>
-      </c>
-    </row>
-    <row r="286" spans="1:3">
-      <c r="A286" t="s">
-        <v>101</v>
-      </c>
-      <c r="B286">
-        <v>40.49</v>
-      </c>
-      <c r="C286" s="2">
-        <v>44744</v>
-      </c>
-    </row>
-    <row r="287" spans="1:3">
-      <c r="A287" t="s">
-        <v>101</v>
-      </c>
-      <c r="B287">
-        <v>52.99</v>
-      </c>
-      <c r="C287" s="2">
-        <v>44835</v>
-      </c>
-    </row>
-    <row r="288" spans="1:3">
-      <c r="A288" t="s">
-        <v>102</v>
-      </c>
-      <c r="B288">
-        <v>31.29</v>
-      </c>
-      <c r="C288" s="2">
-        <v>45024</v>
-      </c>
-    </row>
-    <row r="289" spans="1:3">
-      <c r="A289" t="s">
-        <v>102</v>
-      </c>
-      <c r="B289">
-        <v>25.03</v>
-      </c>
-      <c r="C289" s="2">
-        <v>45066</v>
-      </c>
-    </row>
-    <row r="290" spans="1:3">
-      <c r="A290" t="s">
-        <v>102</v>
-      </c>
-      <c r="B290">
-        <v>156.5</v>
-      </c>
-      <c r="C290" s="2">
-        <v>45073</v>
-      </c>
-    </row>
-    <row r="291" spans="1:3">
-      <c r="A291" t="s">
-        <v>102</v>
-      </c>
-      <c r="B291">
-        <v>860.48</v>
-      </c>
-      <c r="C291" s="2">
-        <v>45073</v>
-      </c>
-    </row>
-    <row r="292" spans="1:3">
-      <c r="A292" t="s">
-        <v>103</v>
-      </c>
-      <c r="B292">
-        <v>45.42</v>
-      </c>
-      <c r="C292" s="2">
-        <v>45038</v>
-      </c>
-    </row>
-    <row r="293" spans="1:3">
-      <c r="A293" t="s">
-        <v>104</v>
-      </c>
-      <c r="B293">
-        <v>26.83</v>
-      </c>
-      <c r="C293" s="2">
-        <v>44954</v>
-      </c>
-    </row>
-    <row r="294" spans="1:3">
-      <c r="A294" t="s">
-        <v>105</v>
-      </c>
-      <c r="B294">
-        <v>26</v>
-      </c>
-      <c r="C294" s="2">
-        <v>44744</v>
-      </c>
-    </row>
-    <row r="295" spans="1:3">
-      <c r="A295" t="s">
-        <v>105</v>
-      </c>
-      <c r="B295">
-        <v>26.73</v>
-      </c>
-      <c r="C295" s="2">
-        <v>44751</v>
-      </c>
-    </row>
-    <row r="296" spans="1:3">
-      <c r="A296" t="s">
-        <v>106</v>
-      </c>
-      <c r="B296">
-        <v>24.06</v>
-      </c>
-      <c r="C296" s="2">
-        <v>44744</v>
-      </c>
-    </row>
-    <row r="297" spans="1:3">
-      <c r="A297" t="s">
-        <v>106</v>
-      </c>
-      <c r="B297">
-        <v>24.61</v>
-      </c>
-      <c r="C297" s="2">
-        <v>44751</v>
-      </c>
-    </row>
-    <row r="298" spans="1:3">
-      <c r="A298" t="s">
-        <v>106</v>
-      </c>
-      <c r="B298">
-        <v>24.83</v>
-      </c>
-      <c r="C298" s="2">
-        <v>44814</v>
-      </c>
-    </row>
-    <row r="299" spans="1:3">
-      <c r="A299" t="s">
-        <v>106</v>
-      </c>
-      <c r="B299">
-        <v>25</v>
-      </c>
-      <c r="C299" s="2">
-        <v>44940</v>
+        <v>45471</v>
       </c>
     </row>
   </sheetData>

</xml_diff>